<commit_message>
trying makespreadsheet, but failed mysteriously
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="1"/>
+    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="105">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Other females (15-49)</t>
   </si>
   <si>
-    <t>Antiretroviral therapy</t>
-  </si>
-  <si>
     <t>high</t>
   </si>
   <si>
@@ -439,6 +436,15 @@
   </si>
   <si>
     <t>F 15-49</t>
+  </si>
+  <si>
+    <t>Unsuppressive ART</t>
+  </si>
+  <si>
+    <t>Suppressive ART</t>
+  </si>
+  <si>
+    <t>Probability of viral suppression on ART</t>
   </si>
 </sst>
 </file>
@@ -2148,7 +2154,7 @@
     </row>
     <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2176,7 +2182,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2223,7 +2229,7 @@
     </row>
     <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2270,7 +2276,7 @@
     </row>
     <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2315,7 +2321,7 @@
     </row>
     <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2348,7 +2354,7 @@
     </row>
     <row r="29" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2394,10 +2400,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2409,25 +2415,25 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="10">
         <v>4.0000000000000002E-4</v>
@@ -2441,7 +2447,7 @@
     </row>
     <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="10">
         <v>8.0000000000000004E-4</v>
@@ -2455,7 +2461,7 @@
     </row>
     <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="10">
         <v>1.38E-2</v>
@@ -2469,7 +2475,7 @@
     </row>
     <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="10">
         <v>1.1000000000000001E-3</v>
@@ -2483,7 +2489,7 @@
     </row>
     <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="10">
         <v>8.0000000000000002E-3</v>
@@ -2497,7 +2503,7 @@
     </row>
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="10">
         <v>0.36699999999999999</v>
@@ -2511,7 +2517,7 @@
     </row>
     <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="10">
         <v>0.20499999999999999</v>
@@ -2534,25 +2540,25 @@
     </row>
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="9">
         <v>26.03</v>
@@ -2566,7 +2572,7 @@
     </row>
     <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
@@ -2580,7 +2586,7 @@
     </row>
     <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="9">
         <v>1</v>
@@ -2594,7 +2600,7 @@
     </row>
     <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="9">
         <v>1</v>
@@ -2608,7 +2614,7 @@
     </row>
     <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="9">
         <v>3.49</v>
@@ -2622,7 +2628,7 @@
     </row>
     <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="9">
         <v>7.17</v>
@@ -2645,25 +2651,25 @@
     </row>
     <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="15">
         <v>4.1399999999999997</v>
@@ -2677,7 +2683,7 @@
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="15">
         <v>1.05</v>
@@ -2691,7 +2697,7 @@
     </row>
     <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="15">
         <v>0.33</v>
@@ -2705,7 +2711,7 @@
     </row>
     <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C29" s="15">
         <v>0.27</v>
@@ -2719,7 +2725,7 @@
     </row>
     <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C30" s="15">
         <v>0.67</v>
@@ -2742,25 +2748,25 @@
     </row>
     <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="15">
         <v>0.45</v>
@@ -2774,7 +2780,7 @@
     </row>
     <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" s="15">
         <v>0.7</v>
@@ -2788,7 +2794,7 @@
     </row>
     <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C38" s="15">
         <v>0.47</v>
@@ -2802,7 +2808,7 @@
     </row>
     <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C39" s="15">
         <v>1.52</v>
@@ -2825,25 +2831,25 @@
     </row>
     <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" s="3"/>
     </row>
     <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
       <c r="C44" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="23">
         <v>3.5999999999999999E-3</v>
@@ -2857,7 +2863,7 @@
     </row>
     <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="23">
         <v>3.5999999999999999E-3</v>
@@ -2871,7 +2877,7 @@
     </row>
     <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C47" s="23">
         <v>5.7999999999999996E-3</v>
@@ -2885,7 +2891,7 @@
     </row>
     <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" s="23">
         <v>8.8000000000000005E-3</v>
@@ -2899,7 +2905,7 @@
     </row>
     <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" s="23">
         <v>5.8999999999999997E-2</v>
@@ -2913,7 +2919,7 @@
     </row>
     <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C50" s="23">
         <v>0.32300000000000001</v>
@@ -2927,7 +2933,7 @@
     </row>
     <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C51" s="23">
         <v>0.23</v>
@@ -2941,7 +2947,7 @@
     </row>
     <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C52" s="23">
         <v>2.17</v>
@@ -2964,34 +2970,33 @@
     </row>
     <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B56" s="3"/>
     </row>
     <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
       <c r="C57" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="C58" s="15">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
       <c r="D58" s="15">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="E58" s="15">
-        <v>0.9</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="G58" s="24"/>
       <c r="H58" s="24"/>
@@ -2999,16 +3004,16 @@
     </row>
     <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C59" s="15">
-        <v>0.9</v>
+        <v>0.58000000000000007</v>
       </c>
       <c r="D59" s="15">
-        <v>0.82000000000000006</v>
+        <v>0.47</v>
       </c>
       <c r="E59" s="15">
-        <v>0.92999999999999994</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="G59" s="24"/>
       <c r="H59" s="24"/>
@@ -3016,16 +3021,16 @@
     </row>
     <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C60" s="15">
-        <v>0.72499999999999998</v>
+        <v>0.54</v>
       </c>
       <c r="D60" s="15">
-        <v>0.65</v>
+        <v>0.32999999999999996</v>
       </c>
       <c r="E60" s="15">
-        <v>0.8</v>
+        <v>0.67999999999999994</v>
       </c>
       <c r="G60" s="24"/>
       <c r="H60" s="24"/>
@@ -3033,16 +3038,16 @@
     </row>
     <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C61" s="15">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="D61" s="15">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E61" s="15">
-        <v>0.97499999999999998</v>
+        <v>0.67999999999999994</v>
       </c>
       <c r="G61" s="24"/>
       <c r="H61" s="24"/>
@@ -3050,16 +3055,16 @@
     </row>
     <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="C62" s="15">
-        <v>0.58000000000000007</v>
+        <v>2.65</v>
       </c>
       <c r="D62" s="15">
-        <v>0.47</v>
+        <v>1.35</v>
       </c>
       <c r="E62" s="15">
-        <v>0.66999999999999993</v>
+        <v>5.19</v>
       </c>
       <c r="G62" s="24"/>
       <c r="H62" s="24"/>
@@ -3070,13 +3075,13 @@
         <v>83</v>
       </c>
       <c r="C63" s="15">
-        <v>0.54</v>
+        <v>0.9</v>
       </c>
       <c r="D63" s="15">
-        <v>0.32999999999999996</v>
+        <v>0.82000000000000006</v>
       </c>
       <c r="E63" s="15">
-        <v>0.67999999999999994</v>
+        <v>0.92999999999999994</v>
       </c>
       <c r="G63" s="24"/>
       <c r="H63" s="24"/>
@@ -3084,16 +3089,16 @@
     </row>
     <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C64" s="15">
-        <v>0</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="D64" s="15">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="E64" s="15">
-        <v>0.67999999999999994</v>
+        <v>0.8</v>
       </c>
       <c r="G64" s="24"/>
       <c r="H64" s="24"/>
@@ -3101,143 +3106,167 @@
     </row>
     <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C65" s="15">
-        <v>2.65</v>
+        <v>0.5</v>
       </c>
       <c r="D65" s="15">
-        <v>1.35</v>
+        <v>0.3</v>
       </c>
       <c r="E65" s="15">
-        <v>5.19</v>
+        <v>0.8</v>
       </c>
       <c r="G65" s="24"/>
       <c r="H65" s="24"/>
       <c r="I65" s="24"/>
     </row>
     <row r="66" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
+      <c r="B66" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C66" s="15">
+        <v>0.92</v>
+      </c>
+      <c r="D66" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="E66" s="15">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="67" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
+      <c r="B67" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C67" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D67" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="E67" s="15">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="68" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-      <c r="C70" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
+    <row r="69" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C71" s="9">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="D71" s="9">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="E71" s="9">
-        <v>0.20499999999999999</v>
-      </c>
+      <c r="A71" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B71" s="3"/>
     </row>
     <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C72" s="9">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D72" s="9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E72" s="9">
-        <v>1.0999999999999999E-2</v>
+      <c r="B72" s="3"/>
+      <c r="C72" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C73" s="9">
-        <v>0.02</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="D73" s="9">
-        <v>1.2999999999999999E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="E73" s="9">
-        <v>2.9000000000000001E-2</v>
+        <v>0.20499999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C74" s="9">
-        <v>7.0000000000000007E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D74" s="9">
-        <v>4.8000000000000001E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E74" s="9">
-        <v>9.4E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C75" s="9">
-        <v>0.26500000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="D75" s="9">
-        <v>0.114</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="E75" s="9">
-        <v>0.47399999999999998</v>
+        <v>2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C76" s="9">
-        <v>0.54700000000000004</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D76" s="9">
-        <v>0.38200000000000001</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E76" s="9">
-        <v>0.71499999999999997</v>
+        <v>9.4E-2</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C77" s="9">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D77" s="9">
+        <v>0.114</v>
+      </c>
+      <c r="E77" s="9">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" s="9">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D78" s="9">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E78" s="9">
+        <v>0.71499999999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" s="9">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="D77" s="9">
+      <c r="D79" s="9">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="E77" s="9">
+      <c r="E79" s="9">
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
@@ -3250,8 +3279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3285,10 +3314,10 @@
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3296,7 +3325,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -3319,7 +3348,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>12</v>
@@ -3509,7 +3538,7 @@
         <v>M 15-49</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -3543,7 +3572,7 @@
       <c r="AG3" s="12"/>
       <c r="AH3" s="12"/>
       <c r="AI3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ3" s="12"/>
     </row>
@@ -3553,7 +3582,7 @@
         <v>M 15-49</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="8">
         <v>525000</v>
@@ -3595,7 +3624,7 @@
       <c r="AG4" s="12"/>
       <c r="AH4" s="12"/>
       <c r="AI4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ4" s="12"/>
     </row>
@@ -3605,7 +3634,7 @@
         <v>M 15-49</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -3639,7 +3668,7 @@
       <c r="AG5" s="12"/>
       <c r="AH5" s="12"/>
       <c r="AI5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ5" s="12"/>
     </row>
@@ -3650,7 +3679,7 @@
         <v>F 15-49</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -3684,7 +3713,7 @@
       <c r="AG7" s="12"/>
       <c r="AH7" s="12"/>
       <c r="AI7" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ7" s="12"/>
     </row>
@@ -3694,7 +3723,7 @@
         <v>F 15-49</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="12">
         <v>626000</v>
@@ -3736,7 +3765,7 @@
       <c r="AG8" s="12"/>
       <c r="AH8" s="12"/>
       <c r="AI8" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ8" s="12"/>
     </row>
@@ -3746,7 +3775,7 @@
         <v>F 15-49</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -3780,7 +3809,7 @@
       <c r="AG9" s="12"/>
       <c r="AH9" s="12"/>
       <c r="AI9" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ9" s="12"/>
     </row>
@@ -3806,7 +3835,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3913,7 +3942,7 @@
         <v>M 15-49</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -3947,7 +3976,7 @@
       <c r="AG3" s="10"/>
       <c r="AH3" s="10"/>
       <c r="AI3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ3" s="10"/>
     </row>
@@ -3957,7 +3986,7 @@
         <v>M 15-49</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10">
@@ -3997,7 +4026,7 @@
       <c r="AG4" s="10"/>
       <c r="AH4" s="10"/>
       <c r="AI4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ4" s="14"/>
     </row>
@@ -4007,7 +4036,7 @@
         <v>M 15-49</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -4041,7 +4070,7 @@
       <c r="AG5" s="10"/>
       <c r="AH5" s="10"/>
       <c r="AI5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ5" s="10"/>
     </row>
@@ -4052,7 +4081,7 @@
         <v>F 15-49</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -4086,7 +4115,7 @@
       <c r="AG7" s="10"/>
       <c r="AH7" s="10"/>
       <c r="AI7" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ7" s="10"/>
     </row>
@@ -4096,7 +4125,7 @@
         <v>F 15-49</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10">
@@ -4136,7 +4165,7 @@
       <c r="AG8" s="10"/>
       <c r="AH8" s="10"/>
       <c r="AI8" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ8" s="10"/>
     </row>
@@ -4146,7 +4175,7 @@
         <v>F 15-49</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -4180,7 +4209,7 @@
       <c r="AG9" s="10"/>
       <c r="AH9" s="10"/>
       <c r="AI9" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ9" s="10"/>
     </row>
@@ -4206,7 +4235,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4348,7 +4377,7 @@
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
       <c r="AH3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI3" s="10"/>
     </row>
@@ -4393,7 +4422,7 @@
       <c r="AF4" s="10"/>
       <c r="AG4" s="10"/>
       <c r="AH4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI4" s="10"/>
     </row>
@@ -4402,7 +4431,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4540,7 +4569,7 @@
       <c r="AF10" s="10"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI10" s="10">
         <v>0.05</v>
@@ -4583,7 +4612,7 @@
       <c r="AF11" s="10"/>
       <c r="AG11" s="10"/>
       <c r="AH11" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI11" s="10">
         <v>0.05</v>
@@ -4594,7 +4623,7 @@
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4734,7 +4763,7 @@
       <c r="AF17" s="10"/>
       <c r="AG17" s="10"/>
       <c r="AH17" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI17" s="10"/>
     </row>
@@ -4777,7 +4806,7 @@
       <c r="AF18" s="10"/>
       <c r="AG18" s="10"/>
       <c r="AH18" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI18" s="10"/>
     </row>
@@ -4803,7 +4832,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4906,7 +4935,7 @@
     </row>
     <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -4940,7 +4969,7 @@
       <c r="AF3" s="9"/>
       <c r="AG3" s="9"/>
       <c r="AH3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI3" s="9"/>
     </row>
@@ -4949,7 +4978,7 @@
     <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5052,7 +5081,7 @@
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -5086,7 +5115,7 @@
       <c r="AF9" s="9"/>
       <c r="AG9" s="9"/>
       <c r="AH9" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI9" s="9"/>
     </row>
@@ -5095,7 +5124,7 @@
     <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5198,7 +5227,7 @@
     </row>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -5232,7 +5261,7 @@
       <c r="AF15" s="9"/>
       <c r="AG15" s="9"/>
       <c r="AH15" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI15" s="9"/>
     </row>
@@ -5241,7 +5270,7 @@
     <row r="18" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5344,7 +5373,7 @@
     </row>
     <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -5378,7 +5407,7 @@
       <c r="AF21" s="9"/>
       <c r="AG21" s="9"/>
       <c r="AH21" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI21" s="9"/>
     </row>
@@ -5387,7 +5416,7 @@
     <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5490,7 +5519,7 @@
     </row>
     <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -5524,7 +5553,7 @@
       <c r="AF27" s="9"/>
       <c r="AG27" s="9"/>
       <c r="AH27" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI27" s="9"/>
     </row>
@@ -5533,7 +5562,7 @@
     <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5636,7 +5665,7 @@
     </row>
     <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -5670,7 +5699,7 @@
       <c r="AF33" s="9"/>
       <c r="AG33" s="9"/>
       <c r="AH33" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI33" s="9"/>
     </row>
@@ -5679,7 +5708,7 @@
     <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5782,7 +5811,7 @@
     </row>
     <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -5816,7 +5845,7 @@
       <c r="AF39" s="9"/>
       <c r="AG39" s="9"/>
       <c r="AH39" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI39" s="9"/>
     </row>
@@ -5840,7 +5869,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5980,7 +6009,7 @@
       <c r="AF3" s="15"/>
       <c r="AG3" s="15"/>
       <c r="AH3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI3" s="15"/>
     </row>
@@ -6023,7 +6052,7 @@
       <c r="AF4" s="15"/>
       <c r="AG4" s="15"/>
       <c r="AH4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI4" s="15"/>
     </row>
@@ -6032,7 +6061,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6135,7 +6164,7 @@
     </row>
     <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -6169,7 +6198,7 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI10" s="16">
         <v>0.65</v>
@@ -6180,7 +6209,7 @@
     <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6283,7 +6312,7 @@
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="6">
         <v>0</v>
@@ -6327,7 +6356,7 @@
       <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>
       <c r="AH16" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI16" s="6"/>
     </row>
@@ -6336,7 +6365,7 @@
     <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6476,7 +6505,7 @@
       <c r="AF22" s="15"/>
       <c r="AG22" s="15"/>
       <c r="AH22" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI22" s="15"/>
     </row>
@@ -6519,7 +6548,7 @@
       <c r="AF23" s="15"/>
       <c r="AG23" s="15"/>
       <c r="AH23" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI23" s="15"/>
     </row>
@@ -6528,7 +6557,7 @@
     <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6631,7 +6660,7 @@
     </row>
     <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -6675,7 +6704,7 @@
       <c r="AF29" s="6"/>
       <c r="AG29" s="6"/>
       <c r="AH29" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI29" s="6"/>
     </row>
@@ -6684,7 +6713,7 @@
     <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6848,7 +6877,7 @@
       <c r="AF35" s="9"/>
       <c r="AG35" s="9"/>
       <c r="AH35" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI35" s="9"/>
     </row>
@@ -6857,7 +6886,7 @@
     <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6960,7 +6989,7 @@
     </row>
     <row r="41" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
@@ -6994,7 +7023,7 @@
       <c r="AF41" s="15"/>
       <c r="AG41" s="15"/>
       <c r="AH41" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI41" s="18">
         <f>14/100*87/100</f>
@@ -7021,7 +7050,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7159,7 +7188,7 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI3" s="17">
         <v>100</v>
@@ -7202,7 +7231,7 @@
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI4" s="17">
         <v>100</v>
@@ -7213,7 +7242,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7351,7 +7380,7 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI10" s="17">
         <f>20%*3*20</f>
@@ -7395,7 +7424,7 @@
       <c r="AF11" s="6"/>
       <c r="AG11" s="6"/>
       <c r="AH11" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI11" s="17">
         <f>10%*3*20</f>
@@ -7407,7 +7436,7 @@
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7545,7 +7574,7 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI17" s="6">
         <v>0</v>
@@ -7588,7 +7617,7 @@
       <c r="AF18" s="6"/>
       <c r="AG18" s="6"/>
       <c r="AH18" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI18" s="6">
         <v>0</v>
@@ -7599,7 +7628,7 @@
     <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7737,7 +7766,7 @@
       <c r="AF24" s="15"/>
       <c r="AG24" s="15"/>
       <c r="AH24" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI24" s="19">
         <v>0.14000000000000001</v>
@@ -7780,7 +7809,7 @@
       <c r="AF25" s="15"/>
       <c r="AG25" s="15"/>
       <c r="AH25" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI25" s="19">
         <v>0.14000000000000001</v>
@@ -7791,7 +7820,7 @@
     <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7929,7 +7958,7 @@
       <c r="AF31" s="15"/>
       <c r="AG31" s="15"/>
       <c r="AH31" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI31" s="15">
         <v>0.3</v>
@@ -7972,7 +8001,7 @@
       <c r="AF32" s="15"/>
       <c r="AG32" s="15"/>
       <c r="AH32" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI32" s="15">
         <v>0.4</v>
@@ -7983,7 +8012,7 @@
     <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8121,7 +8150,7 @@
       <c r="AF38" s="15"/>
       <c r="AG38" s="15"/>
       <c r="AH38" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI38" s="20">
         <v>0</v>
@@ -8164,7 +8193,7 @@
       <c r="AF39" s="15"/>
       <c r="AG39" s="15"/>
       <c r="AH39" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI39" s="19">
         <v>0</v>
@@ -8175,7 +8204,7 @@
     <row r="42" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8313,7 +8342,7 @@
       <c r="AF45" s="15"/>
       <c r="AG45" s="15"/>
       <c r="AH45" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI45" s="19">
         <v>0</v>
@@ -8341,7 +8370,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8479,7 +8508,7 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI3" s="6">
         <v>0</v>
@@ -8522,7 +8551,7 @@
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI4" s="6">
         <v>0</v>
@@ -8533,7 +8562,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8671,7 +8700,7 @@
       <c r="AF10" s="15"/>
       <c r="AG10" s="15"/>
       <c r="AH10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI10" s="15">
         <v>0</v>
@@ -8714,7 +8743,7 @@
       <c r="AF11" s="15"/>
       <c r="AG11" s="15"/>
       <c r="AH11" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI11" s="15">
         <v>0</v>
@@ -8725,7 +8754,7 @@
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8828,7 +8857,7 @@
     </row>
     <row r="17" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -8862,7 +8891,7 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AI17" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
fixed error in makespreadsheet
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="10"/>
+    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -13,11 +13,12 @@
     <sheet name="HIV prevalence" sheetId="15" r:id="rId4"/>
     <sheet name="Other epidemiology" sheetId="6" r:id="rId5"/>
     <sheet name="Optional indicators" sheetId="5" r:id="rId6"/>
-    <sheet name="Testing &amp; treatment" sheetId="7" r:id="rId7"/>
-    <sheet name="Sexual behavior" sheetId="8" r:id="rId8"/>
-    <sheet name="Injecting behavior" sheetId="9" r:id="rId9"/>
-    <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId10"/>
-    <sheet name="Constants" sheetId="12" r:id="rId11"/>
+    <sheet name="Cascade" sheetId="17" r:id="rId7"/>
+    <sheet name="Testing &amp; treatment" sheetId="7" r:id="rId8"/>
+    <sheet name="Sexual behavior" sheetId="8" r:id="rId9"/>
+    <sheet name="Injecting behavior" sheetId="9" r:id="rId10"/>
+    <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId11"/>
+    <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -130,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="112">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -333,9 +334,6 @@
     <t>Acute to CD4(&gt;500)</t>
   </si>
   <si>
-    <t>CD4(350,500) to CD4(200-350)</t>
-  </si>
-  <si>
     <t>CD4(200-350) to CD4(50-200)</t>
   </si>
   <si>
@@ -423,9 +421,6 @@
     <t>STI cofactor increase</t>
   </si>
   <si>
-    <t>Change in transmissibility</t>
-  </si>
-  <si>
     <t>Age from</t>
   </si>
   <si>
@@ -445,6 +440,33 @@
   </si>
   <si>
     <t>Probability of viral suppression on ART</t>
+  </si>
+  <si>
+    <t>CD4(350-500) to CD4(200-350)</t>
+  </si>
+  <si>
+    <t>Changes in transmissibility (%)</t>
+  </si>
+  <si>
+    <t>Immediate linkage to care (%)</t>
+  </si>
+  <si>
+    <t>Linkage to care rate (%/year)</t>
+  </si>
+  <si>
+    <t>Those who stop ART but are still in care (%)</t>
+  </si>
+  <si>
+    <t>Those in care who are then lost to follow-up (%/year)</t>
+  </si>
+  <si>
+    <t>PLHIV lost to follow-up (%/year)</t>
+  </si>
+  <si>
+    <t>Biological failure rate (%/year)</t>
+  </si>
+  <si>
+    <t>ART adherence to viral suppression achieved (%/year)</t>
   </si>
 </sst>
 </file>
@@ -455,10 +477,17 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -526,6 +555,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -572,7 +609,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF18C1FF"/>
+        <fgColor rgb="FFFFC0CB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,162 +645,188 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="104">
+  <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="104"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="104" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="104" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="104" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="8" borderId="2" xfId="104" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="4" fontId="1" fillId="8" borderId="2" xfId="104" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="9" fontId="1" fillId="8" borderId="2" xfId="104" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="104"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="104" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="104" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="104" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="8" borderId="2" xfId="104" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="104">
+  <cellStyles count="105">
     <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Comma 3" xfId="2"/>
     <cellStyle name="Followed Hyperlink 10" xfId="15"/>
@@ -867,6 +930,7 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Normal 3" xfId="6"/>
     <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 5" xfId="104"/>
     <cellStyle name="Percent 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2131,15 +2195,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
+      <c r="A2" s="25"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26"/>
+      <c r="A3" s="25"/>
     </row>
     <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -2154,7 +2218,7 @@
     </row>
     <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2166,6 +2230,556 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="35" width="8.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G2" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J2" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K2" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L2" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M2" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N2" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O2" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P2" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R2" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S2" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T2" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U2" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V2" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W2" s="5">
+        <v>2020</v>
+      </c>
+      <c r="X2" s="5">
+        <v>2021</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>2022</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>2023</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>2024</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>2025</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>2026</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>2027</v>
+      </c>
+      <c r="AE2" s="5">
+        <v>2028</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>2029</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>M 15-49</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F9" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H9" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I9" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J9" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K9" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L9" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M9" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N9" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O9" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P9" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R9" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S9" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T9" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U9" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V9" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W9" s="5">
+        <v>2020</v>
+      </c>
+      <c r="X9" s="5">
+        <v>2021</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>2022</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>2023</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>2024</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>2025</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>2026</v>
+      </c>
+      <c r="AD9" s="5">
+        <v>2027</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>2028</v>
+      </c>
+      <c r="AF9" s="5">
+        <v>2029</v>
+      </c>
+      <c r="AG9" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AI9" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>M 15-49</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="15"/>
+      <c r="AF10" s="15"/>
+      <c r="AG10" s="15"/>
+      <c r="AH10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI10" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="15"/>
+      <c r="AF11" s="15"/>
+      <c r="AG11" s="15"/>
+      <c r="AH11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI11" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F16" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G16" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H16" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I16" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J16" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K16" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L16" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M16" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N16" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O16" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P16" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R16" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S16" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T16" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U16" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V16" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W16" s="5">
+        <v>2020</v>
+      </c>
+      <c r="X16" s="5">
+        <v>2021</v>
+      </c>
+      <c r="Y16" s="5">
+        <v>2022</v>
+      </c>
+      <c r="Z16" s="5">
+        <v>2023</v>
+      </c>
+      <c r="AA16" s="5">
+        <v>2024</v>
+      </c>
+      <c r="AB16" s="5">
+        <v>2025</v>
+      </c>
+      <c r="AC16" s="5">
+        <v>2026</v>
+      </c>
+      <c r="AD16" s="5">
+        <v>2027</v>
+      </c>
+      <c r="AE16" s="5">
+        <v>2028</v>
+      </c>
+      <c r="AF16" s="5">
+        <v>2029</v>
+      </c>
+      <c r="AG16" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AI16" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="6"/>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -2398,12 +3012,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2414,118 +3028,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="29" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="30">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="30">
         <v>1E-4</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="30">
         <v>1.4E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="30">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="30">
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="30">
         <v>1.38E-2</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="30">
         <v>1.0200000000000001E-2</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="30">
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="30">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="30">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="30">
         <v>2.8E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="30">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="30">
         <v>6.3E-3</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="30">
         <v>2.4E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="30">
         <v>0.36699999999999999</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="30">
         <v>0.29399999999999998</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="30">
         <v>0.44</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="30">
         <v>0.20499999999999999</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="30">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="30">
         <v>0.27</v>
       </c>
     </row>
@@ -2539,104 +3164,114 @@
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
     </row>
     <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="5" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="29" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="31">
         <v>26.03</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="31">
         <v>2</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="31">
         <v>48.02</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="31">
         <v>1</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="31">
         <v>1</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="31">
         <v>1</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="31">
         <v>1</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="31">
         <v>1</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="31">
         <v>1</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="31">
         <v>3.49</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="31">
         <v>1.76</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="31">
         <v>6.92</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="31">
         <v>7.17</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="31">
         <v>3.9</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="31">
         <v>12.08</v>
       </c>
     </row>
@@ -2650,90 +3285,99 @@
       <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="5" t="s">
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="29" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="26"/>
+      <c r="B26" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="32">
         <v>4.1399999999999997</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="32">
         <v>2</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="32">
         <v>9.76</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="26"/>
+      <c r="B27" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="32">
         <v>1.05</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="32">
         <v>0.86</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="32">
         <v>1.61</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="26"/>
+      <c r="B28" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="32">
+        <v>0.33</v>
+      </c>
+      <c r="D28" s="32">
+        <v>0.32</v>
+      </c>
+      <c r="E28" s="32">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="15">
-        <v>0.33</v>
-      </c>
-      <c r="D28" s="15">
-        <v>0.32</v>
-      </c>
-      <c r="E28" s="15">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="32">
+        <v>0.27</v>
+      </c>
+      <c r="D29" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="E29" s="32">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="15">
-        <v>0.27</v>
-      </c>
-      <c r="D29" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="E29" s="15">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="15">
+      <c r="C30" s="32">
         <v>0.67</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="32">
         <v>0.44</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="32">
         <v>0.88</v>
       </c>
     </row>
@@ -2747,76 +3391,84 @@
       <c r="B33" s="3"/>
     </row>
     <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+    </row>
+    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="C35" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="32">
+        <v>0.45</v>
+      </c>
+      <c r="D36" s="32">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E36" s="32">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="15">
-        <v>0.45</v>
-      </c>
-      <c r="D36" s="15">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E36" s="15">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="32">
+        <v>0.7</v>
+      </c>
+      <c r="D37" s="32">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E37" s="32">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="26"/>
+      <c r="B38" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="15">
-        <v>0.7</v>
-      </c>
-      <c r="D37" s="15">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="E37" s="15">
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="32">
+        <v>0.47</v>
+      </c>
+      <c r="D38" s="32">
+        <v>0.33</v>
+      </c>
+      <c r="E38" s="32">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
+      <c r="B39" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="15">
-        <v>0.47</v>
-      </c>
-      <c r="D38" s="15">
-        <v>0.33</v>
-      </c>
-      <c r="E38" s="15">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="15">
+      <c r="C39" s="32">
         <v>1.52</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="32">
         <v>1.06</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="32">
         <v>1.96</v>
       </c>
     </row>
@@ -2830,132 +3482,144 @@
       <c r="B42" s="3"/>
     </row>
     <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+    </row>
+    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="26"/>
+      <c r="B45" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="30">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D45" s="30">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="E45" s="30">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="26"/>
+      <c r="B46" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="30">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D46" s="30">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="E46" s="30">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="26"/>
+      <c r="B47" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
-      <c r="C44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="23">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="D45" s="23">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="E45" s="23">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C46" s="23">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="D46" s="23">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="E46" s="23">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+      <c r="C47" s="30">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="D47" s="30">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="E47" s="30">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="26"/>
+      <c r="B48" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="30">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D48" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E48" s="30">
+        <v>1.01E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="26"/>
+      <c r="B49" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="30">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D49" s="30">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E49" s="30">
+        <v>7.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="26"/>
+      <c r="B50" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="30">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="D50" s="30">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="E50" s="30">
+        <v>0.432</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="26"/>
+      <c r="B51" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="23">
-        <v>5.7999999999999996E-3</v>
-      </c>
-      <c r="D47" s="23">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="E47" s="23">
-        <v>7.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="23">
-        <v>8.8000000000000005E-3</v>
-      </c>
-      <c r="D48" s="23">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="E48" s="23">
-        <v>1.01E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" s="23">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="D49" s="23">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="E49" s="23">
-        <v>7.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C50" s="23">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="D50" s="23">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="E50" s="23">
-        <v>0.432</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="30">
+        <v>0.23</v>
+      </c>
+      <c r="D51" s="30">
+        <v>0.15</v>
+      </c>
+      <c r="E51" s="30">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="26"/>
+      <c r="B52" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="23">
-        <v>0.23</v>
-      </c>
-      <c r="D51" s="23">
-        <v>0.15</v>
-      </c>
-      <c r="E51" s="23">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="23">
+      <c r="C52" s="30">
         <v>2.17</v>
       </c>
-      <c r="D52" s="23">
+      <c r="D52" s="30">
         <v>1.27</v>
       </c>
-      <c r="E52" s="23">
+      <c r="E52" s="30">
         <v>3.71</v>
       </c>
     </row>
@@ -2969,183 +3633,198 @@
       <c r="B55" s="3"/>
     </row>
     <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" s="3"/>
+      <c r="A56" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
     </row>
     <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="5" t="s">
+      <c r="A57" s="26"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="29" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+      <c r="A58" s="26"/>
+      <c r="B58" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="32">
+        <v>0.95</v>
+      </c>
+      <c r="D58" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="E58" s="32">
+        <v>0.98</v>
+      </c>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+    </row>
+    <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="26"/>
+      <c r="B59" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="15">
+      <c r="C59" s="32">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D59" s="32">
+        <v>0.47</v>
+      </c>
+      <c r="E59" s="32">
+        <v>0.67</v>
+      </c>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="23"/>
+    </row>
+    <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="26"/>
+      <c r="B60" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="32">
+        <v>0.54</v>
+      </c>
+      <c r="D60" s="32">
+        <v>0.33</v>
+      </c>
+      <c r="E60" s="32">
+        <v>0.68</v>
+      </c>
+      <c r="G60" s="23"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="23"/>
+    </row>
+    <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="26"/>
+      <c r="B61" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" s="32">
+        <v>0</v>
+      </c>
+      <c r="D61" s="32">
+        <v>0</v>
+      </c>
+      <c r="E61" s="32">
+        <v>0.68</v>
+      </c>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+    </row>
+    <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="26"/>
+      <c r="B62" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62" s="32">
+        <v>2.65</v>
+      </c>
+      <c r="D62" s="32">
+        <v>1.35</v>
+      </c>
+      <c r="E62" s="32">
+        <v>5.19</v>
+      </c>
+      <c r="G62" s="23"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="23"/>
+    </row>
+    <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="26"/>
+      <c r="B63" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="32">
+        <v>0.9</v>
+      </c>
+      <c r="D63" s="32">
+        <v>0.82</v>
+      </c>
+      <c r="E63" s="32">
+        <v>0.93</v>
+      </c>
+      <c r="G63" s="23"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
+    </row>
+    <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="26"/>
+      <c r="B64" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" s="32">
+        <v>0.73</v>
+      </c>
+      <c r="D64" s="32">
+        <v>0.65</v>
+      </c>
+      <c r="E64" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="G64" s="23"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
+    </row>
+    <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="26"/>
+      <c r="B65" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="D65" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="E65" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="G65" s="23"/>
+      <c r="H65" s="23"/>
+      <c r="I65" s="23"/>
+    </row>
+    <row r="66" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="26"/>
+      <c r="B66" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C66" s="32">
+        <v>0.92</v>
+      </c>
+      <c r="D66" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="E66" s="32">
         <v>0.95</v>
       </c>
-      <c r="D58" s="15">
+    </row>
+    <row r="67" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="26"/>
+      <c r="B67" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C67" s="32">
+        <v>0.9</v>
+      </c>
+      <c r="D67" s="32">
         <v>0.8</v>
       </c>
-      <c r="E58" s="15">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="G58" s="24"/>
-      <c r="H58" s="24"/>
-      <c r="I58" s="24"/>
-    </row>
-    <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C59" s="15">
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="D59" s="15">
-        <v>0.47</v>
-      </c>
-      <c r="E59" s="15">
-        <v>0.66999999999999993</v>
-      </c>
-      <c r="G59" s="24"/>
-      <c r="H59" s="24"/>
-      <c r="I59" s="24"/>
-    </row>
-    <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C60" s="15">
-        <v>0.54</v>
-      </c>
-      <c r="D60" s="15">
-        <v>0.32999999999999996</v>
-      </c>
-      <c r="E60" s="15">
-        <v>0.67999999999999994</v>
-      </c>
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="24"/>
-    </row>
-    <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C61" s="15">
-        <v>0</v>
-      </c>
-      <c r="D61" s="15">
-        <v>0</v>
-      </c>
-      <c r="E61" s="15">
-        <v>0.67999999999999994</v>
-      </c>
-      <c r="G61" s="24"/>
-      <c r="H61" s="24"/>
-      <c r="I61" s="24"/>
-    </row>
-    <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C62" s="15">
-        <v>2.65</v>
-      </c>
-      <c r="D62" s="15">
-        <v>1.35</v>
-      </c>
-      <c r="E62" s="15">
-        <v>5.19</v>
-      </c>
-      <c r="G62" s="24"/>
-      <c r="H62" s="24"/>
-      <c r="I62" s="24"/>
-    </row>
-    <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C63" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="D63" s="15">
-        <v>0.82000000000000006</v>
-      </c>
-      <c r="E63" s="15">
-        <v>0.92999999999999994</v>
-      </c>
-      <c r="G63" s="24"/>
-      <c r="H63" s="24"/>
-      <c r="I63" s="24"/>
-    </row>
-    <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C64" s="15">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="D64" s="15">
-        <v>0.65</v>
-      </c>
-      <c r="E64" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="G64" s="24"/>
-      <c r="H64" s="24"/>
-      <c r="I64" s="24"/>
-    </row>
-    <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C65" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D65" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="E65" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="G65" s="24"/>
-      <c r="H65" s="24"/>
-      <c r="I65" s="24"/>
-    </row>
-    <row r="66" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C66" s="15">
-        <v>0.92</v>
-      </c>
-      <c r="D66" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="E66" s="15">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C67" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="D67" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="E67" s="15">
+      <c r="E67" s="32">
         <v>0.95</v>
       </c>
     </row>
@@ -3155,118 +3834,129 @@
     <row r="69" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" s="26"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+    </row>
+    <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="26"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="26"/>
+      <c r="B73" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
-      <c r="C72" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+      <c r="C73" s="31">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D73" s="31">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E73" s="31">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="26"/>
+      <c r="B74" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C73" s="9">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="D73" s="9">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="E73" s="9">
-        <v>0.20499999999999999</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+      <c r="C74" s="31">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D74" s="31">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E74" s="31">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="26"/>
+      <c r="B75" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="C74" s="9">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D74" s="9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E74" s="9">
-        <v>1.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
+      <c r="C75" s="31">
+        <v>0.02</v>
+      </c>
+      <c r="D75" s="31">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E75" s="31">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="26"/>
+      <c r="B76" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C75" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="D75" s="9">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E75" s="9">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
+      <c r="C76" s="31">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D76" s="31">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E76" s="31">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="26"/>
+      <c r="B77" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C76" s="9">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D76" s="9">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="E76" s="9">
-        <v>9.4E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+      <c r="C77" s="31">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D77" s="31">
+        <v>0.114</v>
+      </c>
+      <c r="E77" s="31">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="26"/>
+      <c r="B78" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C77" s="9">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="D77" s="9">
-        <v>0.114</v>
-      </c>
-      <c r="E77" s="9">
-        <v>0.47399999999999998</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
+      <c r="C78" s="31">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D78" s="31">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E78" s="31">
+        <v>0.71499999999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="26"/>
+      <c r="B79" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C78" s="9">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="D78" s="9">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="E78" s="9">
-        <v>0.71499999999999997</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C79" s="9">
+      <c r="C79" s="31">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="D79" s="9">
+      <c r="D79" s="31">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="E79" s="9">
+      <c r="E79" s="31">
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
@@ -3314,10 +4004,10 @@
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3325,7 +4015,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -3348,7 +4038,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>12</v>
@@ -4224,8 +4914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI18"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AI3" sqref="AI3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4822,7 +5512,7 @@
   <dimension ref="A1:AI39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5416,7 +6106,7 @@
     <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5855,11 +6545,1167 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+    </row>
+    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D2" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E2" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F2" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G2" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H2" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I2" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J2" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K2" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L2" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M2" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N2" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O2" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P2" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q2" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R2" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S2" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T2" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U2" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V2" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W2" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>M 15-49</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="33"/>
+      <c r="B4" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y4" s="37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="33"/>
+      <c r="W8" s="33"/>
+      <c r="X8" s="33"/>
+      <c r="Y8" s="33"/>
+    </row>
+    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E9" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F9" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G9" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H9" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I9" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J9" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K9" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L9" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M9" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N9" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O9" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P9" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q9" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R9" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S9" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T9" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U9" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V9" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W9" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>M 15-49</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="37"/>
+      <c r="U10" s="37"/>
+      <c r="V10" s="37"/>
+      <c r="W10" s="37"/>
+      <c r="X10" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y10" s="37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="37"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="37"/>
+      <c r="X11" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y11" s="37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="33"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="33"/>
+    </row>
+    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D16" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E16" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F16" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G16" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H16" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I16" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J16" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K16" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L16" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M16" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N16" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O16" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P16" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q16" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R16" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S16" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T16" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U16" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V16" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W16" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X16" s="33"/>
+      <c r="Y16" s="35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
+      <c r="B17" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>M 15-49</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="37"/>
+      <c r="X17" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y17" s="37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
+      <c r="B18" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="37"/>
+      <c r="W18" s="37"/>
+      <c r="X18" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y18" s="37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="33"/>
+      <c r="R22" s="33"/>
+      <c r="S22" s="33"/>
+      <c r="T22" s="33"/>
+      <c r="U22" s="33"/>
+      <c r="V22" s="33"/>
+      <c r="W22" s="33"/>
+      <c r="X22" s="33"/>
+      <c r="Y22" s="33"/>
+    </row>
+    <row r="23" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D23" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E23" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F23" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G23" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H23" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I23" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J23" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K23" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L23" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M23" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N23" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O23" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P23" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q23" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R23" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S23" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T23" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U23" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V23" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W23" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X23" s="33"/>
+      <c r="Y23" s="35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
+      <c r="B24" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>M 15-49</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="37"/>
+      <c r="W24" s="37"/>
+      <c r="X24" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y24" s="37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="33"/>
+      <c r="B25" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y25" s="37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="33"/>
+      <c r="S29" s="33"/>
+      <c r="T29" s="33"/>
+      <c r="U29" s="33"/>
+      <c r="V29" s="33"/>
+      <c r="W29" s="33"/>
+      <c r="X29" s="33"/>
+      <c r="Y29" s="33"/>
+    </row>
+    <row r="30" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D30" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E30" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F30" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G30" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H30" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I30" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J30" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K30" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L30" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M30" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N30" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O30" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P30" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q30" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R30" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S30" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T30" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U30" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V30" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W30" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X30" s="33"/>
+      <c r="Y30" s="35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+      <c r="B31" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>M 15-49</v>
+      </c>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="37"/>
+      <c r="O31" s="37"/>
+      <c r="P31" s="37"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="37"/>
+      <c r="S31" s="37"/>
+      <c r="T31" s="37"/>
+      <c r="U31" s="37"/>
+      <c r="V31" s="37"/>
+      <c r="W31" s="37"/>
+      <c r="X31" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y31" s="37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="37"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="37"/>
+      <c r="T32" s="37"/>
+      <c r="U32" s="37"/>
+      <c r="V32" s="37"/>
+      <c r="W32" s="37"/>
+      <c r="X32" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y32" s="37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="33"/>
+      <c r="Q36" s="33"/>
+      <c r="R36" s="33"/>
+      <c r="S36" s="33"/>
+      <c r="T36" s="33"/>
+      <c r="U36" s="33"/>
+      <c r="V36" s="33"/>
+      <c r="W36" s="33"/>
+      <c r="X36" s="33"/>
+      <c r="Y36" s="33"/>
+    </row>
+    <row r="37" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D37" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E37" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F37" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G37" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H37" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I37" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J37" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K37" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L37" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M37" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N37" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O37" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P37" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q37" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R37" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S37" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T37" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U37" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V37" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W37" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X37" s="33"/>
+      <c r="Y37" s="35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
+      <c r="B38" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>M 15-49</v>
+      </c>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="37"/>
+      <c r="O38" s="37"/>
+      <c r="P38" s="37"/>
+      <c r="Q38" s="37"/>
+      <c r="R38" s="37"/>
+      <c r="S38" s="37"/>
+      <c r="T38" s="37"/>
+      <c r="U38" s="37"/>
+      <c r="V38" s="37"/>
+      <c r="W38" s="37"/>
+      <c r="X38" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y38" s="37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="33"/>
+      <c r="B39" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="37"/>
+      <c r="R39" s="37"/>
+      <c r="S39" s="37"/>
+      <c r="T39" s="37"/>
+      <c r="U39" s="37"/>
+      <c r="V39" s="37"/>
+      <c r="W39" s="37"/>
+      <c r="X39" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y39" s="37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="33"/>
+      <c r="Q43" s="33"/>
+      <c r="R43" s="33"/>
+      <c r="S43" s="33"/>
+      <c r="T43" s="33"/>
+      <c r="U43" s="33"/>
+      <c r="V43" s="33"/>
+      <c r="W43" s="33"/>
+      <c r="X43" s="33"/>
+      <c r="Y43" s="33"/>
+    </row>
+    <row r="44" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="35">
+        <v>2000</v>
+      </c>
+      <c r="D44" s="35">
+        <v>2001</v>
+      </c>
+      <c r="E44" s="35">
+        <v>2002</v>
+      </c>
+      <c r="F44" s="35">
+        <v>2003</v>
+      </c>
+      <c r="G44" s="35">
+        <v>2004</v>
+      </c>
+      <c r="H44" s="35">
+        <v>2005</v>
+      </c>
+      <c r="I44" s="35">
+        <v>2006</v>
+      </c>
+      <c r="J44" s="35">
+        <v>2007</v>
+      </c>
+      <c r="K44" s="35">
+        <v>2008</v>
+      </c>
+      <c r="L44" s="35">
+        <v>2009</v>
+      </c>
+      <c r="M44" s="35">
+        <v>2010</v>
+      </c>
+      <c r="N44" s="35">
+        <v>2011</v>
+      </c>
+      <c r="O44" s="35">
+        <v>2012</v>
+      </c>
+      <c r="P44" s="35">
+        <v>2013</v>
+      </c>
+      <c r="Q44" s="35">
+        <v>2014</v>
+      </c>
+      <c r="R44" s="35">
+        <v>2015</v>
+      </c>
+      <c r="S44" s="35">
+        <v>2016</v>
+      </c>
+      <c r="T44" s="35">
+        <v>2017</v>
+      </c>
+      <c r="U44" s="35">
+        <v>2018</v>
+      </c>
+      <c r="V44" s="35">
+        <v>2019</v>
+      </c>
+      <c r="W44" s="35">
+        <v>2020</v>
+      </c>
+      <c r="X44" s="33"/>
+      <c r="Y44" s="35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="33"/>
+      <c r="B45" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37"/>
+      <c r="O45" s="37"/>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="37"/>
+      <c r="V45" s="37"/>
+      <c r="W45" s="37"/>
+      <c r="X45" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y45" s="37">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B22" sqref="B22:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6209,7 +8055,7 @@
     <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7037,7 +8883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI45"/>
   <sheetViews>
@@ -8353,554 +10199,4 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="35" width="8.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D2" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E2" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F2" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G2" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H2" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I2" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J2" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K2" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L2" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M2" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N2" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O2" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P2" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R2" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S2" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T2" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U2" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V2" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W2" s="5">
-        <v>2020</v>
-      </c>
-      <c r="X2" s="5">
-        <v>2021</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>2022</v>
-      </c>
-      <c r="Z2" s="5">
-        <v>2023</v>
-      </c>
-      <c r="AA2" s="5">
-        <v>2024</v>
-      </c>
-      <c r="AB2" s="5">
-        <v>2025</v>
-      </c>
-      <c r="AC2" s="5">
-        <v>2026</v>
-      </c>
-      <c r="AD2" s="5">
-        <v>2027</v>
-      </c>
-      <c r="AE2" s="5">
-        <v>2028</v>
-      </c>
-      <c r="AF2" s="5">
-        <v>2029</v>
-      </c>
-      <c r="AG2" s="5">
-        <v>2030</v>
-      </c>
-      <c r="AI2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="str">
-        <f>Populations!$C$3</f>
-        <v>M 15-49</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="str">
-        <f>Populations!$C$4</f>
-        <v>F 15-49</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="6"/>
-      <c r="AG4" s="6"/>
-      <c r="AH4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D9" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E9" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F9" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G9" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H9" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I9" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J9" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K9" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L9" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M9" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N9" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O9" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P9" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q9" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R9" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S9" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T9" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U9" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V9" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W9" s="5">
-        <v>2020</v>
-      </c>
-      <c r="X9" s="5">
-        <v>2021</v>
-      </c>
-      <c r="Y9" s="5">
-        <v>2022</v>
-      </c>
-      <c r="Z9" s="5">
-        <v>2023</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>2024</v>
-      </c>
-      <c r="AB9" s="5">
-        <v>2025</v>
-      </c>
-      <c r="AC9" s="5">
-        <v>2026</v>
-      </c>
-      <c r="AD9" s="5">
-        <v>2027</v>
-      </c>
-      <c r="AE9" s="5">
-        <v>2028</v>
-      </c>
-      <c r="AF9" s="5">
-        <v>2029</v>
-      </c>
-      <c r="AG9" s="5">
-        <v>2030</v>
-      </c>
-      <c r="AI9" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="str">
-        <f>Populations!$C$3</f>
-        <v>M 15-49</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="15"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="15"/>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="15"/>
-      <c r="AH10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI10" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="str">
-        <f>Populations!$C$4</f>
-        <v>F 15-49</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="15"/>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="15"/>
-      <c r="AD11" s="15"/>
-      <c r="AE11" s="15"/>
-      <c r="AF11" s="15"/>
-      <c r="AG11" s="15"/>
-      <c r="AH11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI11" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D16" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E16" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F16" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G16" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H16" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I16" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J16" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K16" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L16" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M16" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N16" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O16" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P16" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q16" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R16" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S16" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T16" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U16" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V16" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W16" s="5">
-        <v>2020</v>
-      </c>
-      <c r="X16" s="5">
-        <v>2021</v>
-      </c>
-      <c r="Y16" s="5">
-        <v>2022</v>
-      </c>
-      <c r="Z16" s="5">
-        <v>2023</v>
-      </c>
-      <c r="AA16" s="5">
-        <v>2024</v>
-      </c>
-      <c r="AB16" s="5">
-        <v>2025</v>
-      </c>
-      <c r="AC16" s="5">
-        <v>2026</v>
-      </c>
-      <c r="AD16" s="5">
-        <v>2027</v>
-      </c>
-      <c r="AE16" s="5">
-        <v>2028</v>
-      </c>
-      <c r="AF16" s="5">
-        <v>2029</v>
-      </c>
-      <c r="AG16" s="5">
-        <v>2030</v>
-      </c>
-      <c r="AI16" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="6"/>
-      <c r="X17" s="6"/>
-      <c r="Y17" s="6"/>
-      <c r="Z17" s="6"/>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="6"/>
-      <c r="AE17" s="6"/>
-      <c r="AF17" s="6"/>
-      <c r="AG17" s="6"/>
-      <c r="AH17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
changed adherencerate back to adherenceprop pending confirmation from madhura
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="861" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -20,7 +20,12 @@
     <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -474,8 +479,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -648,9 +653,9 @@
   <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2189,34 +2194,34 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="89.7109375" customWidth="1"/>
+    <col min="1" max="1" width="89.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="12.75" customHeight="1">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="37"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="37"/>
     </row>
-    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="14">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="67.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="14">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="14">
       <c r="A7" s="21" t="s">
         <v>93</v>
       </c>
@@ -2226,6 +2231,11 @@
     <mergeCell ref="A1:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2237,17 +2247,17 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="35" width="8.85546875" customWidth="1"/>
+    <col min="1" max="35" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -2345,7 +2355,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2388,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2431,15 +2441,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:35" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -2537,7 +2547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2580,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2623,15 +2633,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="15" spans="1:35" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -2729,7 +2739,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:35" ht="13.5" customHeight="1">
       <c r="B17" s="22" t="s">
         <v>15</v>
       </c>
@@ -2771,11 +2781,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:35" ht="13.5" customHeight="1"/>
+    <row r="19" spans="2:35" ht="13.5" customHeight="1"/>
+    <row r="20" spans="2:35" ht="13.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2787,21 +2802,21 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13.5" customHeight="1">
       <c r="C2" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2811,7 +2826,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2821,7 +2836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2829,26 +2844,26 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13.5" customHeight="1">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13.5" customHeight="1">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13.5" customHeight="1">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13.5" customHeight="1">
       <c r="C9" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2858,7 +2873,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2868,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2876,26 +2891,26 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="13.5" customHeight="1">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="13.5" customHeight="1">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="13.5" customHeight="1">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1">
       <c r="C16" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2905,7 +2920,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="13.5" customHeight="1">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2913,7 +2928,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="13.5" customHeight="1">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2921,26 +2936,26 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="13.5" customHeight="1">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="13.5" customHeight="1">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="13.5" customHeight="1">
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="13.5" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="13.5" customHeight="1">
       <c r="C23" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2950,7 +2965,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="13.5" customHeight="1">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2958,7 +2973,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="13.5" customHeight="1">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2966,14 +2981,14 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="13.5" customHeight="1">
       <c r="C30" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2983,7 +2998,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="13.5" customHeight="1">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2995,7 +3010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="13.5" customHeight="1">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3009,6 +3024,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3016,18 +3036,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="6" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="6" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1">
       <c r="A1" s="25" t="s">
         <v>50</v>
       </c>
@@ -3036,7 +3056,7 @@
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.5" customHeight="1">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="27" t="s">
@@ -3049,7 +3069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.5" customHeight="1">
       <c r="A3" s="24"/>
       <c r="B3" s="26" t="s">
         <v>51</v>
@@ -3064,7 +3084,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.5" customHeight="1">
       <c r="A4" s="24"/>
       <c r="B4" s="26" t="s">
         <v>52</v>
@@ -3079,7 +3099,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.5" customHeight="1">
       <c r="A5" s="24"/>
       <c r="B5" s="26" t="s">
         <v>53</v>
@@ -3094,7 +3114,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.5" customHeight="1">
       <c r="A6" s="24"/>
       <c r="B6" s="26" t="s">
         <v>54</v>
@@ -3109,7 +3129,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.5" customHeight="1">
       <c r="A7" s="24"/>
       <c r="B7" s="26" t="s">
         <v>55</v>
@@ -3124,7 +3144,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.5" customHeight="1">
       <c r="A8" s="24"/>
       <c r="B8" s="26" t="s">
         <v>56</v>
@@ -3139,7 +3159,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.5" customHeight="1">
       <c r="A9" s="24"/>
       <c r="B9" s="26" t="s">
         <v>57</v>
@@ -3154,16 +3174,16 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.5" customHeight="1">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="13.5" customHeight="1">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="13.5" customHeight="1">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="13.5" customHeight="1">
       <c r="A13" s="25" t="s">
         <v>58</v>
       </c>
@@ -3172,7 +3192,7 @@
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="13.5" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="24"/>
       <c r="C14" s="27" t="s">
@@ -3185,7 +3205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="13.5" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="26" t="s">
         <v>59</v>
@@ -3200,7 +3220,7 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="13.5" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="26" t="s">
         <v>60</v>
@@ -3215,7 +3235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="13.5" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="26" t="s">
         <v>61</v>
@@ -3230,7 +3250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="13.5" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="26" t="s">
         <v>62</v>
@@ -3245,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="13.5" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="26" t="s">
         <v>63</v>
@@ -3260,7 +3280,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="13.5" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="26" t="s">
         <v>64</v>
@@ -3275,16 +3295,16 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="13.5" customHeight="1">
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="13.5" customHeight="1">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="13.5" customHeight="1">
       <c r="A24" s="25" t="s">
         <v>65</v>
       </c>
@@ -3293,7 +3313,7 @@
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
     </row>
-    <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="13.5" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="24"/>
       <c r="C25" s="27" t="s">
@@ -3306,7 +3326,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="13.5" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="26" t="s">
         <v>66</v>
@@ -3321,7 +3341,7 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="13.5" customHeight="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26" t="s">
         <v>61</v>
@@ -3336,7 +3356,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="13.5" customHeight="1">
       <c r="A28" s="24"/>
       <c r="B28" s="26" t="s">
         <v>103</v>
@@ -3351,7 +3371,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="13.5" customHeight="1">
       <c r="A29" s="24"/>
       <c r="B29" s="26" t="s">
         <v>67</v>
@@ -3366,7 +3386,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="13.5" customHeight="1">
       <c r="A30" s="24"/>
       <c r="B30" s="26" t="s">
         <v>68</v>
@@ -3381,16 +3401,16 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="13.5" customHeight="1">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="13.5" customHeight="1">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="13.5" customHeight="1">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="13.5" customHeight="1">
       <c r="A34" s="25" t="s">
         <v>69</v>
       </c>
@@ -3399,7 +3419,7 @@
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
     </row>
-    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="13.5" customHeight="1">
       <c r="A35" s="24"/>
       <c r="B35" s="24"/>
       <c r="C35" s="27" t="s">
@@ -3412,7 +3432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="13.5" customHeight="1">
       <c r="A36" s="24"/>
       <c r="B36" s="26" t="s">
         <v>70</v>
@@ -3427,7 +3447,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="13.5" customHeight="1">
       <c r="A37" s="24"/>
       <c r="B37" s="26" t="s">
         <v>71</v>
@@ -3442,7 +3462,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="13.5" customHeight="1">
       <c r="A38" s="24"/>
       <c r="B38" s="26" t="s">
         <v>72</v>
@@ -3457,7 +3477,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="13.5" customHeight="1">
       <c r="A39" s="24"/>
       <c r="B39" s="26" t="s">
         <v>73</v>
@@ -3472,16 +3492,16 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="13.5" customHeight="1">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="13.5" customHeight="1">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="13.5" customHeight="1">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="13.5" customHeight="1">
       <c r="A43" s="25" t="s">
         <v>74</v>
       </c>
@@ -3490,7 +3510,7 @@
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
     </row>
-    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="13.5" customHeight="1">
       <c r="A44" s="24"/>
       <c r="B44" s="24"/>
       <c r="C44" s="27" t="s">
@@ -3503,7 +3523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="13.5" customHeight="1">
       <c r="A45" s="24"/>
       <c r="B45" s="26" t="s">
         <v>59</v>
@@ -3518,7 +3538,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="13.5" customHeight="1">
       <c r="A46" s="24"/>
       <c r="B46" s="26" t="s">
         <v>60</v>
@@ -3533,7 +3553,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="13.5" customHeight="1">
       <c r="A47" s="24"/>
       <c r="B47" s="26" t="s">
         <v>75</v>
@@ -3548,7 +3568,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="13.5" customHeight="1">
       <c r="A48" s="24"/>
       <c r="B48" s="26" t="s">
         <v>62</v>
@@ -3563,7 +3583,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="13.5" customHeight="1">
       <c r="A49" s="24"/>
       <c r="B49" s="26" t="s">
         <v>63</v>
@@ -3578,7 +3598,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="13.5" customHeight="1">
       <c r="A50" s="24"/>
       <c r="B50" s="26" t="s">
         <v>64</v>
@@ -3593,7 +3613,7 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="13.5" customHeight="1">
       <c r="A51" s="24"/>
       <c r="B51" s="26" t="s">
         <v>76</v>
@@ -3608,7 +3628,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="13.5" customHeight="1">
       <c r="A52" s="24"/>
       <c r="B52" s="26" t="s">
         <v>77</v>
@@ -3623,16 +3643,16 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="13.5" customHeight="1">
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="13.5" customHeight="1">
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="13.5" customHeight="1">
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="13.5" customHeight="1">
       <c r="A56" s="25" t="s">
         <v>104</v>
       </c>
@@ -3641,7 +3661,7 @@
       <c r="D56" s="24"/>
       <c r="E56" s="24"/>
     </row>
-    <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="13.5" customHeight="1">
       <c r="A57" s="24"/>
       <c r="B57" s="24"/>
       <c r="C57" s="27" t="s">
@@ -3654,7 +3674,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="13.5" customHeight="1">
       <c r="A58" s="24"/>
       <c r="B58" s="26" t="s">
         <v>78</v>
@@ -3672,7 +3692,7 @@
       <c r="H58" s="23"/>
       <c r="I58" s="23"/>
     </row>
-    <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="13.5" customHeight="1">
       <c r="A59" s="24"/>
       <c r="B59" s="26" t="s">
         <v>79</v>
@@ -3690,7 +3710,7 @@
       <c r="H59" s="23"/>
       <c r="I59" s="23"/>
     </row>
-    <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="13.5" customHeight="1">
       <c r="A60" s="24"/>
       <c r="B60" s="26" t="s">
         <v>80</v>
@@ -3708,7 +3728,7 @@
       <c r="H60" s="23"/>
       <c r="I60" s="23"/>
     </row>
-    <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="13.5" customHeight="1">
       <c r="A61" s="24"/>
       <c r="B61" s="26" t="s">
         <v>95</v>
@@ -3726,7 +3746,7 @@
       <c r="H61" s="23"/>
       <c r="I61" s="23"/>
     </row>
-    <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="13.5" customHeight="1">
       <c r="A62" s="24"/>
       <c r="B62" s="26" t="s">
         <v>81</v>
@@ -3744,7 +3764,7 @@
       <c r="H62" s="23"/>
       <c r="I62" s="23"/>
     </row>
-    <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="13.5" customHeight="1">
       <c r="A63" s="24"/>
       <c r="B63" s="26" t="s">
         <v>82</v>
@@ -3762,7 +3782,7 @@
       <c r="H63" s="23"/>
       <c r="I63" s="23"/>
     </row>
-    <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="13.5" customHeight="1">
       <c r="A64" s="24"/>
       <c r="B64" s="26" t="s">
         <v>83</v>
@@ -3780,7 +3800,7 @@
       <c r="H64" s="23"/>
       <c r="I64" s="23"/>
     </row>
-    <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="13.5" customHeight="1">
       <c r="A65" s="24"/>
       <c r="B65" s="26" t="s">
         <v>100</v>
@@ -3798,7 +3818,7 @@
       <c r="H65" s="23"/>
       <c r="I65" s="23"/>
     </row>
-    <row r="66" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="13.5" customHeight="1">
       <c r="A66" s="24"/>
       <c r="B66" s="26" t="s">
         <v>101</v>
@@ -3813,7 +3833,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="13.5" customHeight="1">
       <c r="A67" s="24"/>
       <c r="B67" s="26" t="s">
         <v>102</v>
@@ -3828,12 +3848,12 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="13.5" customHeight="1">
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="13.5" customHeight="1"/>
+    <row r="70" spans="1:9" ht="13.5" customHeight="1"/>
+    <row r="71" spans="1:9" ht="13.5" customHeight="1">
       <c r="A71" s="25" t="s">
         <v>84</v>
       </c>
@@ -3842,7 +3862,7 @@
       <c r="D71" s="24"/>
       <c r="E71" s="24"/>
     </row>
-    <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="13.5" customHeight="1">
       <c r="A72" s="24"/>
       <c r="B72" s="24"/>
       <c r="C72" s="27" t="s">
@@ -3855,7 +3875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="13.5" customHeight="1">
       <c r="A73" s="24"/>
       <c r="B73" s="26" t="s">
         <v>85</v>
@@ -3870,7 +3890,7 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="13.5" customHeight="1">
       <c r="A74" s="24"/>
       <c r="B74" s="26" t="s">
         <v>86</v>
@@ -3885,7 +3905,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="13.5" customHeight="1">
       <c r="A75" s="24"/>
       <c r="B75" s="26" t="s">
         <v>87</v>
@@ -3900,7 +3920,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="13.5" customHeight="1">
       <c r="A76" s="24"/>
       <c r="B76" s="26" t="s">
         <v>88</v>
@@ -3915,7 +3935,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="13.5" customHeight="1">
       <c r="A77" s="24"/>
       <c r="B77" s="26" t="s">
         <v>89</v>
@@ -3930,7 +3950,7 @@
         <v>0.47399999999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="15" customHeight="1">
       <c r="A78" s="24"/>
       <c r="B78" s="26" t="s">
         <v>90</v>
@@ -3945,7 +3965,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="15" customHeight="1">
       <c r="A79" s="24"/>
       <c r="B79" s="26" t="s">
         <v>91</v>
@@ -3962,6 +3982,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3973,16 +3998,16 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3990,7 +4015,7 @@
       <c r="D1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.5" customHeight="1">
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -4010,7 +4035,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.5" customHeight="1">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -4033,7 +4058,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.5" customHeight="1">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -4056,53 +4081,58 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.5" customHeight="1">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.5" customHeight="1">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.5" customHeight="1">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.5" customHeight="1">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.5" customHeight="1">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.5" customHeight="1">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.5" customHeight="1">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.5" customHeight="1">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.5" customHeight="1">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="G13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4114,17 +4144,17 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="36" width="8.85546875" customWidth="1"/>
+    <col min="1" max="36" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="13.5" customHeight="1">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -4222,7 +4252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4266,7 +4296,7 @@
       </c>
       <c r="AJ3" s="12"/>
     </row>
-    <row r="4" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4318,7 +4348,7 @@
       </c>
       <c r="AJ4" s="12"/>
     </row>
-    <row r="5" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="13.5" customHeight="1">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4362,8 +4392,8 @@
       </c>
       <c r="AJ5" s="12"/>
     </row>
-    <row r="6" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:36" ht="13.5" customHeight="1">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4407,7 +4437,7 @@
       </c>
       <c r="AJ7" s="12"/>
     </row>
-    <row r="8" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" ht="13.5" customHeight="1">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4459,7 +4489,7 @@
       </c>
       <c r="AJ8" s="12"/>
     </row>
-    <row r="9" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" ht="13.5" customHeight="1">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4503,10 +4533,15 @@
       </c>
       <c r="AJ9" s="12"/>
     </row>
-    <row r="10" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:36" ht="13.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4514,21 +4549,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="36" width="8.85546875" customWidth="1"/>
+    <col min="1" max="36" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="13.5" customHeight="1">
       <c r="D2" s="7">
         <v>2000</v>
       </c>
@@ -4626,7 +4661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4670,7 +4705,7 @@
       </c>
       <c r="AJ3" s="10"/>
     </row>
-    <row r="4" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4720,7 +4755,7 @@
       </c>
       <c r="AJ4" s="14"/>
     </row>
-    <row r="5" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="13.5" customHeight="1">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -4764,8 +4799,8 @@
       </c>
       <c r="AJ5" s="10"/>
     </row>
-    <row r="6" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:36" ht="13.5" customHeight="1">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4809,7 +4844,7 @@
       </c>
       <c r="AJ7" s="10"/>
     </row>
-    <row r="8" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" ht="13.5" customHeight="1">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4859,7 +4894,7 @@
       </c>
       <c r="AJ8" s="10"/>
     </row>
-    <row r="9" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" ht="13.5" customHeight="1">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -4905,8 +4940,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4918,17 +4958,17 @@
       <selection activeCell="C10" sqref="C10:AG11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="35" width="8.85546875" customWidth="1"/>
+    <col min="1" max="35" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -5026,7 +5066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5071,7 +5111,7 @@
       </c>
       <c r="AI3" s="10"/>
     </row>
-    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5116,15 +5156,15 @@
       </c>
       <c r="AI4" s="10"/>
     </row>
-    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:35" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -5222,7 +5262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5265,7 +5305,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5308,15 +5348,15 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="15" spans="1:35" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -5414,7 +5454,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:35" ht="13.5" customHeight="1">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5457,7 +5497,7 @@
       </c>
       <c r="AI17" s="10"/>
     </row>
-    <row r="18" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:35" ht="13.5" customHeight="1">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5504,6 +5544,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5515,17 +5560,17 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="35" width="8.85546875" customWidth="1"/>
+    <col min="1" max="35" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -5623,7 +5668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="13.5" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
@@ -5663,15 +5708,15 @@
       </c>
       <c r="AI3" s="9"/>
     </row>
-    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="5" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:35" ht="13.5" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="13.5" customHeight="1">
       <c r="C8" s="5">
         <v>2000</v>
       </c>
@@ -5769,7 +5814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="13.5" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
@@ -5809,15 +5854,15 @@
       </c>
       <c r="AI9" s="9"/>
     </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="11" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="12" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:35" ht="13.5" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="13.5" customHeight="1">
       <c r="C14" s="5">
         <v>2000</v>
       </c>
@@ -5915,7 +5960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="13.5" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
@@ -5955,15 +6000,15 @@
       </c>
       <c r="AI15" s="9"/>
     </row>
-    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="17" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="18" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="19" spans="1:35" ht="13.5" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="13.5" customHeight="1">
       <c r="C20" s="5">
         <v>2000</v>
       </c>
@@ -6061,7 +6106,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="13.5" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>15</v>
       </c>
@@ -6101,15 +6146,15 @@
       </c>
       <c r="AI21" s="9"/>
     </row>
-    <row r="22" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="23" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="24" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="25" spans="1:35" ht="13.5" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="13.5" customHeight="1">
       <c r="C26" s="7">
         <v>2000</v>
       </c>
@@ -6207,7 +6252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" ht="13.5" customHeight="1">
       <c r="B27" s="7" t="s">
         <v>15</v>
       </c>
@@ -6247,15 +6292,15 @@
       </c>
       <c r="AI27" s="9"/>
     </row>
-    <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="29" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="30" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="31" spans="1:35" ht="13.5" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="13.5" customHeight="1">
       <c r="C32" s="5">
         <v>2000</v>
       </c>
@@ -6353,7 +6398,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" ht="13.5" customHeight="1">
       <c r="B33" s="5" t="s">
         <v>15</v>
       </c>
@@ -6393,15 +6438,15 @@
       </c>
       <c r="AI33" s="9"/>
     </row>
-    <row r="34" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="35" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="36" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="37" spans="1:35" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="13.5" customHeight="1">
       <c r="C38" s="5">
         <v>2000</v>
       </c>
@@ -6499,7 +6544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="13.5" customHeight="1">
       <c r="B39" s="5" t="s">
         <v>15</v>
       </c>
@@ -6541,6 +6586,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6548,13 +6598,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="14">
       <c r="A1" s="32" t="s">
         <v>105</v>
       </c>
@@ -6593,7 +6643,7 @@
       <c r="AH1" s="31"/>
       <c r="AI1" s="31"/>
     </row>
-    <row r="2" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="14">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="33">
@@ -6694,7 +6744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="14">
       <c r="A3" s="31"/>
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -6738,7 +6788,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="14">
       <c r="A4" s="31"/>
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -6782,7 +6832,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="14">
       <c r="A8" s="32" t="s">
         <v>106</v>
       </c>
@@ -6821,7 +6871,7 @@
       <c r="AH8" s="31"/>
       <c r="AI8" s="31"/>
     </row>
-    <row r="9" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="14">
       <c r="A9" s="31"/>
       <c r="B9" s="31"/>
       <c r="C9" s="33">
@@ -6922,7 +6972,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="14">
       <c r="A10" s="31"/>
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -6966,7 +7016,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="14">
       <c r="A11" s="31"/>
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -7010,7 +7060,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="14">
       <c r="A15" s="32" t="s">
         <v>111</v>
       </c>
@@ -7049,7 +7099,7 @@
       <c r="AH15" s="31"/>
       <c r="AI15" s="31"/>
     </row>
-    <row r="16" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="14">
       <c r="A16" s="31"/>
       <c r="B16" s="31"/>
       <c r="C16" s="33">
@@ -7150,7 +7200,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="14">
       <c r="A17" s="31"/>
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -7194,7 +7244,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="14">
       <c r="A18" s="31"/>
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -7238,7 +7288,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="14">
       <c r="A22" s="32" t="s">
         <v>107</v>
       </c>
@@ -7277,7 +7327,7 @@
       <c r="AH22" s="31"/>
       <c r="AI22" s="31"/>
     </row>
-    <row r="23" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="14">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
       <c r="C23" s="33">
@@ -7378,7 +7428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="14">
       <c r="A24" s="31"/>
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -7422,7 +7472,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="14">
       <c r="A25" s="31"/>
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -7466,7 +7516,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" ht="14">
       <c r="A29" s="32" t="s">
         <v>108</v>
       </c>
@@ -7505,7 +7555,7 @@
       <c r="AH29" s="31"/>
       <c r="AI29" s="31"/>
     </row>
-    <row r="30" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="14">
       <c r="A30" s="31"/>
       <c r="B30" s="31"/>
       <c r="C30" s="33">
@@ -7606,7 +7656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" ht="14">
       <c r="A31" s="31"/>
       <c r="B31" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -7650,7 +7700,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="14">
       <c r="A32" s="31"/>
       <c r="B32" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -7694,7 +7744,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" ht="14">
       <c r="A36" s="32" t="s">
         <v>109</v>
       </c>
@@ -7733,7 +7783,7 @@
       <c r="AH36" s="31"/>
       <c r="AI36" s="31"/>
     </row>
-    <row r="37" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" ht="14">
       <c r="A37" s="31"/>
       <c r="B37" s="31"/>
       <c r="C37" s="33">
@@ -7834,7 +7884,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="14">
       <c r="A38" s="31"/>
       <c r="B38" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -7878,7 +7928,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="14">
       <c r="A39" s="31"/>
       <c r="B39" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -7922,7 +7972,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" ht="14">
       <c r="A43" s="32" t="s">
         <v>110</v>
       </c>
@@ -7961,7 +8011,7 @@
       <c r="AH43" s="31"/>
       <c r="AI43" s="31"/>
     </row>
-    <row r="44" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" ht="14">
       <c r="A44" s="31"/>
       <c r="B44" s="31"/>
       <c r="C44" s="33">
@@ -8062,7 +8112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" ht="14">
       <c r="A45" s="31"/>
       <c r="B45" s="33" t="s">
         <v>31</v>
@@ -8107,6 +8157,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8114,21 +8169,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B22" sqref="B22:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="35" width="8.85546875" customWidth="1"/>
+    <col min="1" max="35" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -8226,7 +8281,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8269,7 +8324,7 @@
       </c>
       <c r="AI3" s="15"/>
     </row>
-    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8312,15 +8367,15 @@
       </c>
       <c r="AI4" s="15"/>
     </row>
-    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:35" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -8418,7 +8473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="13.5" customHeight="1">
       <c r="B10" s="5" t="s">
         <v>31</v>
       </c>
@@ -8460,15 +8515,15 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="12" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:35" ht="13.5" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="13.5" customHeight="1">
       <c r="C15" s="5">
         <v>2000</v>
       </c>
@@ -8566,7 +8621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="13.5" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
@@ -8616,15 +8671,15 @@
       </c>
       <c r="AI16" s="6"/>
     </row>
-    <row r="17" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="18" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="19" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="20" spans="1:35" ht="13.5" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="13.5" customHeight="1">
       <c r="C21" s="5">
         <v>2000</v>
       </c>
@@ -8722,7 +8777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="13.5" customHeight="1">
       <c r="B22" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8765,7 +8820,7 @@
       </c>
       <c r="AI22" s="15"/>
     </row>
-    <row r="23" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="13.5" customHeight="1">
       <c r="B23" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8808,15 +8863,15 @@
       </c>
       <c r="AI23" s="15"/>
     </row>
-    <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="25" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="26" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="27" spans="1:35" ht="13.5" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" ht="13.5" customHeight="1">
       <c r="C28" s="5">
         <v>2000</v>
       </c>
@@ -8914,7 +8969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" ht="13.5" customHeight="1">
       <c r="B29" s="5" t="s">
         <v>15</v>
       </c>
@@ -8964,15 +9019,15 @@
       </c>
       <c r="AI29" s="6"/>
     </row>
-    <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="31" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="32" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="33" spans="1:35" ht="13.5" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" ht="13.5" customHeight="1">
       <c r="C34" s="5">
         <v>2000</v>
       </c>
@@ -9070,7 +9125,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" ht="13.5" customHeight="1">
       <c r="B35" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9137,15 +9192,15 @@
       </c>
       <c r="AI35" s="9"/>
     </row>
-    <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="37" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="38" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="39" spans="1:35" ht="13.5" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="13.5" customHeight="1">
       <c r="C40" s="5">
         <v>2000</v>
       </c>
@@ -9243,7 +9298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" ht="13.5" customHeight="1">
       <c r="B41" s="5" t="s">
         <v>15</v>
       </c>
@@ -9290,6 +9345,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9297,19 +9357,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="V36" workbookViewId="0">
+      <selection activeCell="AI46" sqref="AI46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="35" width="8.85546875" customWidth="1"/>
+    <col min="1" max="35" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="13.5" customHeight="1">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -9407,7 +9469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="13.5" customHeight="1">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9450,7 +9512,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="13.5" customHeight="1">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9493,15 +9555,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="6" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="7" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="8" spans="1:35" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="13.5" customHeight="1">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -9599,7 +9661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="13.5" customHeight="1">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9643,7 +9705,7 @@
         <v>12.000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="13.5" customHeight="1">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9687,15 +9749,15 @@
         <v>6.0000000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="13" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="15" spans="1:35" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="13.5" customHeight="1">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -9793,7 +9855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="13.5" customHeight="1">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9836,7 +9898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="13.5" customHeight="1">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9879,15 +9941,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="20" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="21" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="22" spans="1:35" ht="13.5" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="13.5" customHeight="1">
       <c r="C23" s="5">
         <v>2000</v>
       </c>
@@ -9985,7 +10047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="13.5" customHeight="1">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -10028,7 +10090,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="13.5" customHeight="1">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -10071,15 +10133,15 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="27" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="28" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="29" spans="1:35" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="13.5" customHeight="1">
       <c r="C30" s="5">
         <v>2000</v>
       </c>
@@ -10177,7 +10239,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" ht="13.5" customHeight="1">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -10220,7 +10282,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="13.5" customHeight="1">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -10263,15 +10325,15 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="34" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="35" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="36" spans="1:35" ht="13.5" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" ht="13.5" customHeight="1">
       <c r="C37" s="5">
         <v>2000</v>
       </c>
@@ -10369,7 +10431,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="13.5" customHeight="1">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -10412,7 +10474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="13.5" customHeight="1">
       <c r="B39" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -10455,15 +10517,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="41" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="42" spans="1:35" ht="13.5" customHeight="1"/>
+    <row r="43" spans="1:35" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" ht="13.5" customHeight="1">
       <c r="C44" s="5">
         <v>2000</v>
       </c>
@@ -10561,7 +10623,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" ht="13.5" customHeight="1">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -10601,12 +10663,17 @@
         <v>16</v>
       </c>
       <c r="AI45" s="19">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
quick fix to spreadsheet text
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="861" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14715" tabRatio="861"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -141,9 +141,6 @@
     <t>O P T I M A</t>
   </si>
   <si>
-    <t>Welcome to the Optima data entry spreadsheet. This is where all data for the model will be entered. At first glance the spreadsheet looks complicated and confusing. Unfortunately, it is. So please ask someone from the Optima development team if you need help, or use the default contact (info@optimamodel.com).</t>
-  </si>
-  <si>
     <t>Populations</t>
   </si>
   <si>
@@ -472,6 +469,9 @@
   </si>
   <si>
     <t>ART adherence to viral suppression achieved (%/year)</t>
+  </si>
+  <si>
+    <t>Welcome to the Optima data entry spreadsheet. This is where all data for the model will be entered. At first glance the spreadsheet may look complicated. So please ask someone from the Optima development team if you need help, or use the default contact (info@optimamodel.com).</t>
   </si>
 </sst>
 </file>
@@ -479,8 +479,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -653,9 +653,9 @@
   <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2190,40 +2190,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="89.6640625" customWidth="1"/>
+    <col min="1" max="1" width="89.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="12.75" customHeight="1">
+    <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="37"/>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
     </row>
-    <row r="4" spans="1:1" ht="14">
+    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" ht="67.5" customHeight="1">
+    <row r="5" spans="1:1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="14">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" ht="14">
+    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2247,17 +2247,17 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="35" width="8.83203125" customWidth="1"/>
+    <col min="1" max="35" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="13.5" customHeight="1">
+    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" ht="13.5" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -2352,10 +2352,10 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2392,13 +2392,13 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI3" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="13.5" customHeight="1">
+    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2435,21 +2435,21 @@
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI4" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="6" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="8" spans="1:35" ht="13.5" customHeight="1">
+    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -2544,10 +2544,10 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2584,13 +2584,13 @@
       <c r="AF10" s="15"/>
       <c r="AG10" s="15"/>
       <c r="AH10" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI10" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1">
+    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2627,21 +2627,21 @@
       <c r="AF11" s="15"/>
       <c r="AG11" s="15"/>
       <c r="AH11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI11" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="13" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="14" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="15" spans="1:35" ht="13.5" customHeight="1">
+    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" ht="13.5" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -2736,12 +2736,12 @@
         <v>2030</v>
       </c>
       <c r="AI16" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="2:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2775,15 +2775,15 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI17" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:35" ht="13.5" customHeight="1"/>
-    <row r="19" spans="2:35" ht="13.5" customHeight="1"/>
-    <row r="20" spans="2:35" ht="13.5" customHeight="1"/>
+    <row r="18" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2802,21 +2802,21 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="6" width="8.83203125" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" customHeight="1">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1">
+    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2826,7 +2826,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1">
+    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2836,7 +2836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5" customHeight="1">
+    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2844,26 +2844,26 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="13.5" customHeight="1">
+    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1">
+    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1">
+    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="13.5" customHeight="1">
+    <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="13.5" customHeight="1">
+    <row r="9" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2873,7 +2873,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5" customHeight="1">
+    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2883,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2891,26 +2891,26 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="13.5" customHeight="1">
+    <row r="12" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="13.5" customHeight="1">
+    <row r="13" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="13.5" customHeight="1">
+    <row r="14" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="13.5" customHeight="1">
+    <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1">
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2920,7 +2920,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13.5" customHeight="1">
+    <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2928,7 +2928,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="13.5" customHeight="1">
+    <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2936,26 +2936,26 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="13.5" customHeight="1">
+    <row r="19" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="13.5" customHeight="1">
+    <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="13.5" customHeight="1">
+    <row r="21" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="13.5" customHeight="1">
+    <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="13.5" customHeight="1">
+    <row r="23" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2965,7 +2965,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="13.5" customHeight="1">
+    <row r="24" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2973,7 +2973,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="13.5" customHeight="1">
+    <row r="25" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -2981,14 +2981,14 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="13.5" customHeight="1">
+    <row r="29" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="13.5" customHeight="1">
+    <row r="30" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -2998,7 +2998,7 @@
         <v>F 15-49</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="13.5" customHeight="1">
+    <row r="31" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -3010,7 +3010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="13.5" customHeight="1">
+    <row r="32" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -3040,39 +3040,39 @@
       <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="6" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1">
+    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="28">
         <v>4.0000000000000002E-4</v>
@@ -3084,10 +3084,10 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1">
+    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="28">
         <v>8.0000000000000004E-4</v>
@@ -3099,10 +3099,10 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1">
+    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="28">
         <v>1.38E-2</v>
@@ -3114,10 +3114,10 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1">
+    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="28">
         <v>1.1000000000000001E-3</v>
@@ -3129,10 +3129,10 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1">
+    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="28">
         <v>8.0000000000000002E-3</v>
@@ -3144,10 +3144,10 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1">
+    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="28">
         <v>0.36699999999999999</v>
@@ -3159,10 +3159,10 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1">
+    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="28">
         <v>0.20499999999999999</v>
@@ -3174,41 +3174,41 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1">
+    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1">
+    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1">
+    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1">
+    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1">
+    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="24"/>
       <c r="C14" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="29">
         <v>26.03</v>
@@ -3220,10 +3220,10 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1">
+    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="29">
         <v>1</v>
@@ -3235,10 +3235,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="13.5" customHeight="1">
+    <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="29">
         <v>1</v>
@@ -3250,10 +3250,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="13.5" customHeight="1">
+    <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="29">
         <v>1</v>
@@ -3265,10 +3265,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="13.5" customHeight="1">
+    <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="29">
         <v>3.49</v>
@@ -3280,10 +3280,10 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="13.5" customHeight="1">
+    <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="29">
         <v>7.17</v>
@@ -3295,41 +3295,41 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="13.5" customHeight="1">
+    <row r="21" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="13.5" customHeight="1">
+    <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="13.5" customHeight="1">
+    <row r="23" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="13.5" customHeight="1">
+    <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
     </row>
-    <row r="25" spans="1:5" ht="13.5" customHeight="1">
+    <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="24"/>
       <c r="C25" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="13.5" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="30">
         <v>4.1399999999999997</v>
@@ -3341,10 +3341,10 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1">
+    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="30">
         <v>1.05</v>
@@ -3356,10 +3356,10 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13.5" customHeight="1">
+    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
       <c r="B28" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" s="30">
         <v>0.33</v>
@@ -3371,10 +3371,10 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="13.5" customHeight="1">
+    <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
       <c r="B29" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="30">
         <v>0.27</v>
@@ -3386,10 +3386,10 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="13.5" customHeight="1">
+    <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="30">
         <v>0.67</v>
@@ -3401,41 +3401,41 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="13.5" customHeight="1">
+    <row r="31" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="13.5" customHeight="1">
+    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1">
+    <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="13.5" customHeight="1">
+    <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
     </row>
-    <row r="35" spans="1:5" ht="13.5" customHeight="1">
+    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24"/>
       <c r="B35" s="24"/>
       <c r="C35" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="30">
         <v>0.45</v>
@@ -3447,10 +3447,10 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1">
+    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
       <c r="B37" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C37" s="30">
         <v>0.7</v>
@@ -3462,10 +3462,10 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1">
+    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24"/>
       <c r="B38" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" s="30">
         <v>0.47</v>
@@ -3477,10 +3477,10 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1">
+    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
       <c r="B39" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" s="30">
         <v>1.52</v>
@@ -3492,41 +3492,41 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1">
+    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1">
+    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1">
+    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1">
+    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B43" s="24"/>
       <c r="C43" s="24"/>
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
     </row>
-    <row r="44" spans="1:5" ht="13.5" customHeight="1">
+    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="24"/>
       <c r="B44" s="24"/>
       <c r="C44" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="13.5" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="24"/>
       <c r="B45" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" s="28">
         <v>3.5999999999999999E-3</v>
@@ -3538,10 +3538,10 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="13.5" customHeight="1">
+    <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="24"/>
       <c r="B46" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46" s="28">
         <v>3.5999999999999999E-3</v>
@@ -3553,10 +3553,10 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="13.5" customHeight="1">
+    <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24"/>
       <c r="B47" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C47" s="28">
         <v>5.7999999999999996E-3</v>
@@ -3568,10 +3568,10 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="13.5" customHeight="1">
+    <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="24"/>
       <c r="B48" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C48" s="28">
         <v>8.8000000000000005E-3</v>
@@ -3583,10 +3583,10 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="13.5" customHeight="1">
+    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24"/>
       <c r="B49" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49" s="28">
         <v>5.8999999999999997E-2</v>
@@ -3598,10 +3598,10 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="13.5" customHeight="1">
+    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="24"/>
       <c r="B50" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" s="28">
         <v>0.32300000000000001</v>
@@ -3613,10 +3613,10 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="13.5" customHeight="1">
+    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="24"/>
       <c r="B51" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C51" s="28">
         <v>0.23</v>
@@ -3628,10 +3628,10 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="13.5" customHeight="1">
+    <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="24"/>
       <c r="B52" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" s="28">
         <v>2.17</v>
@@ -3643,41 +3643,41 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="13.5" customHeight="1">
+    <row r="53" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:9" ht="13.5" customHeight="1">
+    <row r="54" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:9" ht="13.5" customHeight="1">
+    <row r="55" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:9" ht="13.5" customHeight="1">
+    <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B56" s="24"/>
       <c r="C56" s="24"/>
       <c r="D56" s="24"/>
       <c r="E56" s="24"/>
     </row>
-    <row r="57" spans="1:9" ht="13.5" customHeight="1">
+    <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
       <c r="B57" s="24"/>
       <c r="C57" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E57" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="13.5" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="24"/>
       <c r="B58" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" s="30">
         <v>0.95</v>
@@ -3692,10 +3692,10 @@
       <c r="H58" s="23"/>
       <c r="I58" s="23"/>
     </row>
-    <row r="59" spans="1:9" ht="13.5" customHeight="1">
+    <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="24"/>
       <c r="B59" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C59" s="30">
         <v>0.57999999999999996</v>
@@ -3710,10 +3710,10 @@
       <c r="H59" s="23"/>
       <c r="I59" s="23"/>
     </row>
-    <row r="60" spans="1:9" ht="13.5" customHeight="1">
+    <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="24"/>
       <c r="B60" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C60" s="30">
         <v>0.54</v>
@@ -3728,10 +3728,10 @@
       <c r="H60" s="23"/>
       <c r="I60" s="23"/>
     </row>
-    <row r="61" spans="1:9" ht="13.5" customHeight="1">
+    <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24"/>
       <c r="B61" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C61" s="30">
         <v>0</v>
@@ -3746,10 +3746,10 @@
       <c r="H61" s="23"/>
       <c r="I61" s="23"/>
     </row>
-    <row r="62" spans="1:9" ht="13.5" customHeight="1">
+    <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="24"/>
       <c r="B62" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C62" s="30">
         <v>2.65</v>
@@ -3764,10 +3764,10 @@
       <c r="H62" s="23"/>
       <c r="I62" s="23"/>
     </row>
-    <row r="63" spans="1:9" ht="13.5" customHeight="1">
+    <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24"/>
       <c r="B63" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C63" s="30">
         <v>0.9</v>
@@ -3782,10 +3782,10 @@
       <c r="H63" s="23"/>
       <c r="I63" s="23"/>
     </row>
-    <row r="64" spans="1:9" ht="13.5" customHeight="1">
+    <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24"/>
       <c r="B64" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C64" s="30">
         <v>0.73</v>
@@ -3800,10 +3800,10 @@
       <c r="H64" s="23"/>
       <c r="I64" s="23"/>
     </row>
-    <row r="65" spans="1:9" ht="13.5" customHeight="1">
+    <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="24"/>
       <c r="B65" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C65" s="30">
         <v>0.5</v>
@@ -3818,10 +3818,10 @@
       <c r="H65" s="23"/>
       <c r="I65" s="23"/>
     </row>
-    <row r="66" spans="1:9" ht="13.5" customHeight="1">
+    <row r="66" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="24"/>
       <c r="B66" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C66" s="30">
         <v>0.92</v>
@@ -3833,10 +3833,10 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="13.5" customHeight="1">
+    <row r="67" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="24"/>
       <c r="B67" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C67" s="30">
         <v>0.9</v>
@@ -3848,37 +3848,37 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="13.5" customHeight="1">
+    <row r="68" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:9" ht="13.5" customHeight="1"/>
-    <row r="70" spans="1:9" ht="13.5" customHeight="1"/>
-    <row r="71" spans="1:9" ht="13.5" customHeight="1">
+    <row r="69" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B71" s="24"/>
       <c r="C71" s="24"/>
       <c r="D71" s="24"/>
       <c r="E71" s="24"/>
     </row>
-    <row r="72" spans="1:9" ht="13.5" customHeight="1">
+    <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="24"/>
       <c r="B72" s="24"/>
       <c r="C72" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D72" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E72" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="13.5" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="24"/>
       <c r="B73" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C73" s="29">
         <v>0.14599999999999999</v>
@@ -3890,10 +3890,10 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="13.5" customHeight="1">
+    <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="24"/>
       <c r="B74" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C74" s="29">
         <v>8.0000000000000002E-3</v>
@@ -3905,10 +3905,10 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="13.5" customHeight="1">
+    <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24"/>
       <c r="B75" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C75" s="29">
         <v>0.02</v>
@@ -3920,10 +3920,10 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="13.5" customHeight="1">
+    <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="24"/>
       <c r="B76" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C76" s="29">
         <v>7.0000000000000007E-2</v>
@@ -3935,10 +3935,10 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="13.5" customHeight="1">
+    <row r="77" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="24"/>
       <c r="B77" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C77" s="29">
         <v>0.26500000000000001</v>
@@ -3950,10 +3950,10 @@
         <v>0.47399999999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15" customHeight="1">
+    <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="24"/>
       <c r="B78" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C78" s="29">
         <v>0.54700000000000004</v>
@@ -3965,10 +3965,10 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15" customHeight="1">
+    <row r="79" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="24"/>
       <c r="B79" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C79" s="29">
         <v>5.2999999999999999E-2</v>
@@ -3998,58 +3998,58 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" customWidth="1"/>
-    <col min="5" max="6" width="8.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" customHeight="1">
+    <row r="1" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="13.5" customHeight="1">
+    <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="G2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="13.5" customHeight="1">
+    </row>
+    <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="G3" s="6">
         <v>15</v>
@@ -4058,21 +4058,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.5" customHeight="1">
+    <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="6">
         <v>15</v>
@@ -4081,47 +4081,47 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1">
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="13.5" customHeight="1">
+    <row r="6" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="13.5" customHeight="1">
+    <row r="7" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" customHeight="1">
+    <row r="8" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" customHeight="1">
+    <row r="9" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" customHeight="1">
+    <row r="10" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" customHeight="1">
+    <row r="11" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" customHeight="1">
+    <row r="12" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" customHeight="1">
+    <row r="13" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="G13" s="3"/>
@@ -4144,17 +4144,17 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="36" width="8.83203125" customWidth="1"/>
+    <col min="1" max="36" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="13.5" customHeight="1">
+    <row r="1" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" ht="13.5" customHeight="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -4249,16 +4249,16 @@
         <v>2030</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -4292,17 +4292,17 @@
       <c r="AG3" s="12"/>
       <c r="AH3" s="12"/>
       <c r="AI3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ3" s="12"/>
     </row>
-    <row r="4" spans="1:36" ht="13.5" customHeight="1">
+    <row r="4" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="8">
         <v>525000</v>
@@ -4344,17 +4344,17 @@
       <c r="AG4" s="12"/>
       <c r="AH4" s="12"/>
       <c r="AI4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ4" s="12"/>
     </row>
-    <row r="5" spans="1:36" ht="13.5" customHeight="1">
+    <row r="5" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -4388,18 +4388,18 @@
       <c r="AG5" s="12"/>
       <c r="AH5" s="12"/>
       <c r="AI5" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ5" s="12"/>
     </row>
-    <row r="6" spans="1:36" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:36" ht="13.5" customHeight="1">
+    <row r="6" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -4433,17 +4433,17 @@
       <c r="AG7" s="12"/>
       <c r="AH7" s="12"/>
       <c r="AI7" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ7" s="12"/>
     </row>
-    <row r="8" spans="1:36" ht="13.5" customHeight="1">
+    <row r="8" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="12">
         <v>626000</v>
@@ -4485,17 +4485,17 @@
       <c r="AG8" s="12"/>
       <c r="AH8" s="12"/>
       <c r="AI8" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ8" s="12"/>
     </row>
-    <row r="9" spans="1:36" ht="13.5" customHeight="1">
+    <row r="9" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -4529,11 +4529,11 @@
       <c r="AG9" s="12"/>
       <c r="AH9" s="12"/>
       <c r="AI9" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ9" s="12"/>
     </row>
-    <row r="10" spans="1:36" ht="13.5" customHeight="1"/>
+    <row r="10" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4553,17 +4553,17 @@
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="36" width="8.83203125" customWidth="1"/>
+    <col min="1" max="36" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="13.5" customHeight="1">
+    <row r="1" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" ht="13.5" customHeight="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="7">
         <v>2000</v>
       </c>
@@ -4658,16 +4658,16 @@
         <v>2030</v>
       </c>
       <c r="AJ2" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -4701,17 +4701,17 @@
       <c r="AG3" s="10"/>
       <c r="AH3" s="10"/>
       <c r="AI3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ3" s="10"/>
     </row>
-    <row r="4" spans="1:36" ht="13.5" customHeight="1">
+    <row r="4" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10">
@@ -4751,17 +4751,17 @@
       <c r="AG4" s="10"/>
       <c r="AH4" s="10"/>
       <c r="AI4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ4" s="14"/>
     </row>
-    <row r="5" spans="1:36" ht="13.5" customHeight="1">
+    <row r="5" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -4795,18 +4795,18 @@
       <c r="AG5" s="10"/>
       <c r="AH5" s="10"/>
       <c r="AI5" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ5" s="10"/>
     </row>
-    <row r="6" spans="1:36" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:36" ht="13.5" customHeight="1">
+    <row r="6" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -4840,17 +4840,17 @@
       <c r="AG7" s="10"/>
       <c r="AH7" s="10"/>
       <c r="AI7" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ7" s="10"/>
     </row>
-    <row r="8" spans="1:36" ht="13.5" customHeight="1">
+    <row r="8" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10">
@@ -4890,17 +4890,17 @@
       <c r="AG8" s="10"/>
       <c r="AH8" s="10"/>
       <c r="AI8" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ8" s="10"/>
     </row>
-    <row r="9" spans="1:36" ht="13.5" customHeight="1">
+    <row r="9" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -4934,7 +4934,7 @@
       <c r="AG9" s="10"/>
       <c r="AH9" s="10"/>
       <c r="AI9" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ9" s="10"/>
     </row>
@@ -4958,17 +4958,17 @@
       <selection activeCell="C10" sqref="C10:AG11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="35" width="8.83203125" customWidth="1"/>
+    <col min="1" max="35" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="13.5" customHeight="1">
+    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" ht="13.5" customHeight="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -5063,10 +5063,10 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5107,11 +5107,11 @@
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
       <c r="AH3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI3" s="10"/>
     </row>
-    <row r="4" spans="1:35" ht="13.5" customHeight="1">
+    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5152,19 +5152,19 @@
       <c r="AF4" s="10"/>
       <c r="AG4" s="10"/>
       <c r="AH4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI4" s="10"/>
     </row>
-    <row r="5" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="6" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="8" spans="1:35" ht="13.5" customHeight="1">
+    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -5259,10 +5259,10 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5299,13 +5299,13 @@
       <c r="AF10" s="10"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI10" s="10">
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1">
+    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5342,21 +5342,21 @@
       <c r="AF11" s="10"/>
       <c r="AG11" s="10"/>
       <c r="AH11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI11" s="10">
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="13" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="14" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="15" spans="1:35" ht="13.5" customHeight="1">
+    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" ht="13.5" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -5451,10 +5451,10 @@
         <v>2030</v>
       </c>
       <c r="AI16" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="2:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -5493,11 +5493,11 @@
       <c r="AF17" s="10"/>
       <c r="AG17" s="10"/>
       <c r="AH17" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI17" s="10"/>
     </row>
-    <row r="18" spans="2:35" ht="13.5" customHeight="1">
+    <row r="18" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -5536,7 +5536,7 @@
       <c r="AF18" s="10"/>
       <c r="AG18" s="10"/>
       <c r="AH18" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI18" s="10"/>
     </row>
@@ -5560,17 +5560,17 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="35" width="8.83203125" customWidth="1"/>
+    <col min="1" max="35" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="13.5" customHeight="1">
+    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" ht="13.5" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -5665,12 +5665,12 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -5704,19 +5704,19 @@
       <c r="AF3" s="9"/>
       <c r="AG3" s="9"/>
       <c r="AH3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI3" s="9"/>
+    </row>
+    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="9"/>
-    </row>
-    <row r="4" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="5" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="6" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:35" ht="13.5" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" ht="13.5" customHeight="1">
+    </row>
+    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="5">
         <v>2000</v>
       </c>
@@ -5811,12 +5811,12 @@
         <v>2030</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -5850,19 +5850,19 @@
       <c r="AF9" s="9"/>
       <c r="AG9" s="9"/>
       <c r="AH9" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI9" s="9"/>
     </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="12" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="13" spans="1:35" ht="13.5" customHeight="1">
+    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" ht="13.5" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="5">
         <v>2000</v>
       </c>
@@ -5957,12 +5957,12 @@
         <v>2030</v>
       </c>
       <c r="AI14" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -5996,19 +5996,19 @@
       <c r="AF15" s="9"/>
       <c r="AG15" s="9"/>
       <c r="AH15" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI15" s="9"/>
     </row>
-    <row r="16" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="17" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="18" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="19" spans="1:35" ht="13.5" customHeight="1">
+    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:35" ht="13.5" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="5">
         <v>2000</v>
       </c>
@@ -6103,12 +6103,12 @@
         <v>2030</v>
       </c>
       <c r="AI20" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -6142,19 +6142,19 @@
       <c r="AF21" s="9"/>
       <c r="AG21" s="9"/>
       <c r="AH21" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI21" s="9"/>
     </row>
-    <row r="22" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="23" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="24" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="25" spans="1:35" ht="13.5" customHeight="1">
+    <row r="22" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35" ht="13.5" customHeight="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7">
         <v>2000</v>
       </c>
@@ -6249,12 +6249,12 @@
         <v>2030</v>
       </c>
       <c r="AI26" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -6288,19 +6288,19 @@
       <c r="AF27" s="9"/>
       <c r="AG27" s="9"/>
       <c r="AH27" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI27" s="9"/>
     </row>
-    <row r="28" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="29" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="30" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="31" spans="1:35" ht="13.5" customHeight="1">
+    <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:35" ht="13.5" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="5">
         <v>2000</v>
       </c>
@@ -6395,12 +6395,12 @@
         <v>2030</v>
       </c>
       <c r="AI32" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -6434,19 +6434,19 @@
       <c r="AF33" s="9"/>
       <c r="AG33" s="9"/>
       <c r="AH33" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI33" s="9"/>
     </row>
-    <row r="34" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="35" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="36" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="37" spans="1:35" ht="13.5" customHeight="1">
+    <row r="34" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:35" ht="13.5" customHeight="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="5">
         <v>2000</v>
       </c>
@@ -6541,12 +6541,12 @@
         <v>2030</v>
       </c>
       <c r="AI38" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -6580,7 +6580,7 @@
       <c r="AF39" s="9"/>
       <c r="AG39" s="9"/>
       <c r="AH39" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI39" s="9"/>
     </row>
@@ -6602,11 +6602,11 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:35" ht="14">
+    <row r="1" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -6643,7 +6643,7 @@
       <c r="AH1" s="31"/>
       <c r="AI1" s="31"/>
     </row>
-    <row r="2" spans="1:35" ht="14">
+    <row r="2" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="33">
@@ -6741,10 +6741,10 @@
       </c>
       <c r="AH2" s="31"/>
       <c r="AI2" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -6782,13 +6782,13 @@
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
       <c r="AH3" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI3" s="35">
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="14">
+    <row r="4" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -6826,15 +6826,15 @@
       <c r="AF4" s="10"/>
       <c r="AG4" s="10"/>
       <c r="AH4" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI4" s="35">
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="14">
+    <row r="8" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
@@ -6871,7 +6871,7 @@
       <c r="AH8" s="31"/>
       <c r="AI8" s="31"/>
     </row>
-    <row r="9" spans="1:35" ht="14">
+    <row r="9" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="31"/>
       <c r="C9" s="33">
@@ -6969,10 +6969,10 @@
       </c>
       <c r="AH9" s="31"/>
       <c r="AI9" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -7010,13 +7010,13 @@
       <c r="AF10" s="10"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI10" s="35">
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="14">
+    <row r="11" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -7054,15 +7054,15 @@
       <c r="AF11" s="10"/>
       <c r="AG11" s="10"/>
       <c r="AH11" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI11" s="35">
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="14">
+    <row r="15" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
@@ -7099,7 +7099,7 @@
       <c r="AH15" s="31"/>
       <c r="AI15" s="31"/>
     </row>
-    <row r="16" spans="1:35" ht="14">
+    <row r="16" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
       <c r="B16" s="31"/>
       <c r="C16" s="33">
@@ -7197,10 +7197,10 @@
       </c>
       <c r="AH16" s="31"/>
       <c r="AI16" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:35" ht="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -7238,13 +7238,13 @@
       <c r="AF17" s="10"/>
       <c r="AG17" s="10"/>
       <c r="AH17" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI17" s="35">
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="14">
+    <row r="18" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -7282,15 +7282,15 @@
       <c r="AF18" s="10"/>
       <c r="AG18" s="10"/>
       <c r="AH18" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI18" s="35">
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="14">
+    <row r="22" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
@@ -7327,7 +7327,7 @@
       <c r="AH22" s="31"/>
       <c r="AI22" s="31"/>
     </row>
-    <row r="23" spans="1:35" ht="14">
+    <row r="23" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
       <c r="C23" s="33">
@@ -7425,10 +7425,10 @@
       </c>
       <c r="AH23" s="31"/>
       <c r="AI23" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" ht="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -7466,13 +7466,13 @@
       <c r="AF24" s="10"/>
       <c r="AG24" s="10"/>
       <c r="AH24" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI24" s="35">
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="14">
+    <row r="25" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -7510,15 +7510,15 @@
       <c r="AF25" s="10"/>
       <c r="AG25" s="10"/>
       <c r="AH25" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI25" s="35">
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="14">
+    <row r="29" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B29" s="31"/>
       <c r="C29" s="31"/>
@@ -7555,7 +7555,7 @@
       <c r="AH29" s="31"/>
       <c r="AI29" s="31"/>
     </row>
-    <row r="30" spans="1:35" ht="14">
+    <row r="30" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="B30" s="31"/>
       <c r="C30" s="33">
@@ -7653,10 +7653,10 @@
       </c>
       <c r="AH30" s="31"/>
       <c r="AI30" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:35" ht="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="B31" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -7694,13 +7694,13 @@
       <c r="AF31" s="10"/>
       <c r="AG31" s="10"/>
       <c r="AH31" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI31" s="35">
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="14">
+    <row r="32" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="B32" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -7738,15 +7738,15 @@
       <c r="AF32" s="10"/>
       <c r="AG32" s="10"/>
       <c r="AH32" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI32" s="35">
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:35" ht="14">
+    <row r="36" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36" s="31"/>
       <c r="C36" s="31"/>
@@ -7783,7 +7783,7 @@
       <c r="AH36" s="31"/>
       <c r="AI36" s="31"/>
     </row>
-    <row r="37" spans="1:35" ht="14">
+    <row r="37" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="B37" s="31"/>
       <c r="C37" s="33">
@@ -7881,10 +7881,10 @@
       </c>
       <c r="AH37" s="31"/>
       <c r="AI37" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:35" ht="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -7922,13 +7922,13 @@
       <c r="AF38" s="10"/>
       <c r="AG38" s="10"/>
       <c r="AH38" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI38" s="35">
         <v>0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="14">
+    <row r="39" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -7966,15 +7966,15 @@
       <c r="AF39" s="10"/>
       <c r="AG39" s="10"/>
       <c r="AH39" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI39" s="35">
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="1:35" ht="14">
+    <row r="43" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" s="31"/>
       <c r="C43" s="31"/>
@@ -8011,7 +8011,7 @@
       <c r="AH43" s="31"/>
       <c r="AI43" s="31"/>
     </row>
-    <row r="44" spans="1:35" ht="14">
+    <row r="44" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="31"/>
       <c r="B44" s="31"/>
       <c r="C44" s="33">
@@ -8109,13 +8109,13 @@
       </c>
       <c r="AH44" s="31"/>
       <c r="AI44" s="33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:35" ht="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" s="35"/>
       <c r="D45" s="35"/>
@@ -8149,7 +8149,7 @@
       <c r="AF45" s="35"/>
       <c r="AG45" s="35"/>
       <c r="AH45" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI45" s="35">
         <v>0.1</v>
@@ -8173,17 +8173,17 @@
       <selection activeCell="B22" sqref="B22:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="35" width="8.83203125" customWidth="1"/>
+    <col min="1" max="35" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="13.5" customHeight="1">
+    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" ht="13.5" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -8278,10 +8278,10 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8320,11 +8320,11 @@
       <c r="AF3" s="15"/>
       <c r="AG3" s="15"/>
       <c r="AH3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI3" s="15"/>
     </row>
-    <row r="4" spans="1:35" ht="13.5" customHeight="1">
+    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8363,19 +8363,19 @@
       <c r="AF4" s="15"/>
       <c r="AG4" s="15"/>
       <c r="AH4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI4" s="15"/>
     </row>
-    <row r="5" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="6" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="8" spans="1:35" ht="13.5" customHeight="1">
+    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -8470,12 +8470,12 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -8509,21 +8509,21 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI10" s="16">
         <v>0.65</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="12" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="13" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="14" spans="1:35" ht="13.5" customHeight="1">
+    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" ht="13.5" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="5">
         <v>2000</v>
       </c>
@@ -8618,12 +8618,12 @@
         <v>2030</v>
       </c>
       <c r="AI15" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="6">
         <v>0</v>
@@ -8667,19 +8667,19 @@
       <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>
       <c r="AH16" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI16" s="6"/>
     </row>
-    <row r="17" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="18" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="19" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="20" spans="1:35" ht="13.5" customHeight="1">
+    <row r="17" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:35" ht="13.5" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="5">
         <v>2000</v>
       </c>
@@ -8774,10 +8774,10 @@
         <v>2030</v>
       </c>
       <c r="AI21" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -8816,11 +8816,11 @@
       <c r="AF22" s="15"/>
       <c r="AG22" s="15"/>
       <c r="AH22" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI22" s="15"/>
     </row>
-    <row r="23" spans="1:35" ht="13.5" customHeight="1">
+    <row r="23" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -8859,19 +8859,19 @@
       <c r="AF23" s="15"/>
       <c r="AG23" s="15"/>
       <c r="AH23" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI23" s="15"/>
     </row>
-    <row r="24" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="25" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="26" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="27" spans="1:35" ht="13.5" customHeight="1">
+    <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:35" ht="13.5" customHeight="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="5">
         <v>2000</v>
       </c>
@@ -8966,12 +8966,12 @@
         <v>2030</v>
       </c>
       <c r="AI28" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -9015,19 +9015,19 @@
       <c r="AF29" s="6"/>
       <c r="AG29" s="6"/>
       <c r="AH29" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI29" s="6"/>
     </row>
-    <row r="30" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="31" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="32" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="33" spans="1:35" ht="13.5" customHeight="1">
+    <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:35" ht="13.5" customHeight="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="5">
         <v>2000</v>
       </c>
@@ -9122,10 +9122,10 @@
         <v>2030</v>
       </c>
       <c r="AI34" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9188,19 +9188,19 @@
       <c r="AF35" s="9"/>
       <c r="AG35" s="9"/>
       <c r="AH35" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI35" s="9"/>
     </row>
-    <row r="36" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="37" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="38" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="39" spans="1:35" ht="13.5" customHeight="1">
+    <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:35" ht="13.5" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="5">
         <v>2000</v>
       </c>
@@ -9295,12 +9295,12 @@
         <v>2030</v>
       </c>
       <c r="AI40" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
@@ -9334,7 +9334,7 @@
       <c r="AF41" s="15"/>
       <c r="AG41" s="15"/>
       <c r="AH41" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI41" s="18">
         <f>14/100*87/100</f>
@@ -9357,21 +9357,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V36" workbookViewId="0">
-      <selection activeCell="AI46" sqref="AI46"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="35" width="8.83203125" customWidth="1"/>
+    <col min="1" max="35" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="13.5" customHeight="1">
+    <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" ht="13.5" customHeight="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -9466,10 +9464,10 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9506,13 +9504,13 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI3" s="17">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="13.5" customHeight="1">
+    <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9549,21 +9547,21 @@
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI4" s="17">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="6" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="7" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="8" spans="1:35" ht="13.5" customHeight="1">
+    <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" ht="13.5" customHeight="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5">
         <v>2000</v>
       </c>
@@ -9658,10 +9656,10 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9698,14 +9696,14 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI10" s="17">
         <f>20%*3*20</f>
         <v>12.000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="13.5" customHeight="1">
+    <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9742,22 +9740,22 @@
       <c r="AF11" s="6"/>
       <c r="AG11" s="6"/>
       <c r="AH11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI11" s="17">
         <f>10%*3*20</f>
         <v>6.0000000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="13" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="14" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="15" spans="1:35" ht="13.5" customHeight="1">
+    <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" ht="13.5" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5">
         <v>2000</v>
       </c>
@@ -9852,10 +9850,10 @@
         <v>2030</v>
       </c>
       <c r="AI16" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -9892,13 +9890,13 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI17" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="13.5" customHeight="1">
+    <row r="18" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -9935,21 +9933,21 @@
       <c r="AF18" s="6"/>
       <c r="AG18" s="6"/>
       <c r="AH18" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI18" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="20" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="21" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="22" spans="1:35" ht="13.5" customHeight="1">
+    <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:35" ht="13.5" customHeight="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="5">
         <v>2000</v>
       </c>
@@ -10044,10 +10042,10 @@
         <v>2030</v>
       </c>
       <c r="AI23" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -10084,13 +10082,13 @@
       <c r="AF24" s="15"/>
       <c r="AG24" s="15"/>
       <c r="AH24" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI24" s="19">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="13.5" customHeight="1">
+    <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -10127,21 +10125,21 @@
       <c r="AF25" s="15"/>
       <c r="AG25" s="15"/>
       <c r="AH25" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI25" s="19">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="27" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="28" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="29" spans="1:35" ht="13.5" customHeight="1">
+    <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:35" ht="13.5" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
         <v>2000</v>
       </c>
@@ -10236,10 +10234,10 @@
         <v>2030</v>
       </c>
       <c r="AI30" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -10276,13 +10274,13 @@
       <c r="AF31" s="15"/>
       <c r="AG31" s="15"/>
       <c r="AH31" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI31" s="15">
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="13.5" customHeight="1">
+    <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -10319,21 +10317,21 @@
       <c r="AF32" s="15"/>
       <c r="AG32" s="15"/>
       <c r="AH32" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI32" s="15">
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="34" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="35" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="36" spans="1:35" ht="13.5" customHeight="1">
+    <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:35" ht="13.5" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="5">
         <v>2000</v>
       </c>
@@ -10428,10 +10426,10 @@
         <v>2030</v>
       </c>
       <c r="AI37" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -10468,13 +10466,13 @@
       <c r="AF38" s="15"/>
       <c r="AG38" s="15"/>
       <c r="AH38" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI38" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="13.5" customHeight="1">
+    <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
@@ -10511,21 +10509,21 @@
       <c r="AF39" s="15"/>
       <c r="AG39" s="15"/>
       <c r="AH39" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI39" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="41" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="42" spans="1:35" ht="13.5" customHeight="1"/>
-    <row r="43" spans="1:35" ht="13.5" customHeight="1">
+    <row r="40" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:35" ht="13.5" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="5">
         <v>2000</v>
       </c>
@@ -10620,10 +10618,10 @@
         <v>2030</v>
       </c>
       <c r="AI44" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:35" ht="13.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
@@ -10660,7 +10658,7 @@
       <c r="AF45" s="15"/>
       <c r="AG45" s="15"/>
       <c r="AH45" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI45" s="19">
         <v>0.1</v>

</xml_diff>

<commit_message>
change spreadsheets and fix mistake in last commit
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="861" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="861" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="114">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -472,6 +472,12 @@
   </si>
   <si>
     <t>Percentage of people in care who are lost to follow-up per year (%/year)</t>
+  </si>
+  <si>
+    <t>Injects</t>
+  </si>
+  <si>
+    <t>Sex worker</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -568,6 +574,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -650,7 +668,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -756,6 +774,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -831,9 +851,10 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="105">
+  <cellStyles count="107">
     <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Comma 3" xfId="2"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="15"/>
     <cellStyle name="Followed Hyperlink 11" xfId="16"/>
     <cellStyle name="Followed Hyperlink 12" xfId="17"/>
@@ -931,6 +952,7 @@
     <cellStyle name="Followed Hyperlink 96" xfId="101"/>
     <cellStyle name="Followed Hyperlink 97" xfId="102"/>
     <cellStyle name="Followed Hyperlink 98" xfId="103"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Normal 3" xfId="6"/>
@@ -3992,10 +4014,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -4007,7 +4029,7 @@
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" customHeight="1">
+    <row r="1" spans="1:10" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -4015,7 +4037,7 @@
       <c r="D1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="13.5" customHeight="1">
+    <row r="2" spans="1:10" ht="13.5" customHeight="1">
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
@@ -4034,8 +4056,14 @@
       <c r="H2" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="13.5" customHeight="1">
+      <c r="I2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="13.5" customHeight="1">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -4057,8 +4085,14 @@
       <c r="H3" s="6">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="13.5" customHeight="1">
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="13.5" customHeight="1">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -4080,54 +4114,61 @@
       <c r="H4" s="6">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1">
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="13.5" customHeight="1">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="13.5" customHeight="1">
+    <row r="6" spans="1:10" ht="13.5" customHeight="1">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="13.5" customHeight="1">
+    <row r="7" spans="1:10" ht="13.5" customHeight="1">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" customHeight="1">
+    <row r="8" spans="1:10" ht="13.5" customHeight="1">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" customHeight="1">
+    <row r="9" spans="1:10" ht="13.5" customHeight="1">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" customHeight="1">
+    <row r="10" spans="1:10" ht="13.5" customHeight="1">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" customHeight="1">
+    <row r="11" spans="1:10" ht="13.5" customHeight="1">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" customHeight="1">
+    <row r="12" spans="1:10" ht="13.5" customHeight="1">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" customHeight="1">
+    <row r="13" spans="1:10" ht="13.5" customHeight="1">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="G13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6598,7 +6639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed bug in transmissability change constants
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="861" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="861" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -482,7 +482,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -568,6 +568,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -650,7 +662,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -756,6 +768,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -831,9 +845,10 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="105">
+  <cellStyles count="107">
     <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Comma 3" xfId="2"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="15"/>
     <cellStyle name="Followed Hyperlink 11" xfId="16"/>
     <cellStyle name="Followed Hyperlink 12" xfId="17"/>
@@ -931,6 +946,7 @@
     <cellStyle name="Followed Hyperlink 96" xfId="101"/>
     <cellStyle name="Followed Hyperlink 97" xfId="102"/>
     <cellStyle name="Followed Hyperlink 98" xfId="103"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Normal 3" xfId="6"/>
@@ -3036,8 +3052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -3716,10 +3732,10 @@
         <v>79</v>
       </c>
       <c r="C60" s="30">
-        <v>0.54</v>
+        <v>0</v>
       </c>
       <c r="D60" s="30">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="E60" s="30">
         <v>0.68</v>
@@ -3734,13 +3750,13 @@
         <v>94</v>
       </c>
       <c r="C61" s="30">
-        <v>0</v>
+        <v>2.65</v>
       </c>
       <c r="D61" s="30">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E61" s="30">
-        <v>0.68</v>
+        <v>5.19</v>
       </c>
       <c r="G61" s="23"/>
       <c r="H61" s="23"/>
@@ -3752,13 +3768,13 @@
         <v>80</v>
       </c>
       <c r="C62" s="30">
-        <v>2.65</v>
+        <v>0.54</v>
       </c>
       <c r="D62" s="30">
-        <v>1.35</v>
+        <v>0.33</v>
       </c>
       <c r="E62" s="30">
-        <v>5.19</v>
+        <v>0.68</v>
       </c>
       <c r="G62" s="23"/>
       <c r="H62" s="23"/>
@@ -3982,6 +3998,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6598,7 +6615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
done first part, not sure how to proceed
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="861" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="861" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="115">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -478,6 +478,9 @@
   </si>
   <si>
     <t>Sex worker</t>
+  </si>
+  <si>
+    <t>Births</t>
   </si>
 </sst>
 </file>
@@ -668,7 +671,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -776,6 +779,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -851,10 +856,11 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="109">
     <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Comma 3" xfId="2"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="15"/>
     <cellStyle name="Followed Hyperlink 11" xfId="16"/>
     <cellStyle name="Followed Hyperlink 12" xfId="17"/>
@@ -953,6 +959,7 @@
     <cellStyle name="Followed Hyperlink 97" xfId="102"/>
     <cellStyle name="Followed Hyperlink 98" xfId="103"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Normal 3" xfId="6"/>
@@ -2818,10 +2825,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -3005,7 +3012,7 @@
     </row>
     <row r="29" spans="1:4" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>48</v>
+        <v>114</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -3022,30 +3029,56 @@
     </row>
     <row r="31" spans="1:4" ht="13.5" customHeight="1">
       <c r="B31" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="35" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" ht="13.5" customHeight="1">
+      <c r="C36" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C31" s="6">
-        <v>0</v>
-      </c>
-      <c r="D31" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="13.5" customHeight="1">
-      <c r="B32" s="7" t="str">
+      <c r="D36" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C32" s="6">
+    </row>
+    <row r="37" spans="1:4" ht="13.5" customHeight="1">
+      <c r="B37" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>M 15-49</v>
+      </c>
+      <c r="C37" s="6">
         <v>0</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D37" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="13.5" customHeight="1">
+      <c r="B38" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>F 15-49</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4017,7 +4050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>

</xml_diff>